<commit_message>
actualizacion para evitar cierre de sesiones admin
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Guia</t>
   </si>
@@ -231,25 +231,16 @@
     <t>INTERRAPIDISIMO</t>
   </si>
   <si>
-    <t>EP-TA800XBEGCA</t>
-  </si>
-  <si>
-    <t>000CA25702</t>
-  </si>
-  <si>
-    <t>ACS00427</t>
-  </si>
-  <si>
-    <t>FXXI0029</t>
-  </si>
-  <si>
-    <t>FSHW0040</t>
-  </si>
-  <si>
-    <t>ASSG0002</t>
-  </si>
-  <si>
-    <t>XDXI0018</t>
+    <t>1829-2</t>
+  </si>
+  <si>
+    <t>ACS01637</t>
+  </si>
+  <si>
+    <t>INTERRAPIDISIMO - CONTADO</t>
+  </si>
+  <si>
+    <t>FMAP0011</t>
   </si>
 </sst>
 </file>
@@ -408,7 +399,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -416,6 +407,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -446,16 +457,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -769,11 +770,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,20 +868,18 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>999064414037</v>
-      </c>
+      <c r="A2" s="8"/>
       <c r="B2" s="1">
-        <v>4286732494</v>
+        <v>1829</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -919,7 +918,7 @@
       </c>
       <c r="U2" s="1">
         <f t="shared" ref="U2" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="V2" s="1">
         <f t="shared" ref="V2" si="1">VLOOKUP(G2,T_TIPO_ENVIO,2,FALSE)</f>
@@ -927,20 +926,17 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>999064416669</v>
-      </c>
       <c r="B3" s="1">
-        <v>1852</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="1">
+        <v>1829</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -948,8 +944,6 @@
       <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
       <c r="K3" s="1">
         <v>1</v>
       </c>
@@ -975,330 +969,39 @@
         <v>33</v>
       </c>
       <c r="S3" s="1">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="T3" s="1"/>
       <c r="U3" s="1">
-        <f t="shared" ref="U3:U4" si="2">VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
-        <v>1</v>
+        <f t="shared" ref="U3" si="2">VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
+        <v>5</v>
       </c>
       <c r="V3" s="1">
-        <f t="shared" ref="V3:V4" si="3">VLOOKUP(G3,T_TIPO_ENVIO,2,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>999064416755</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1851</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1">
-        <v>17</v>
-      </c>
-      <c r="N4" s="1">
-        <v>20</v>
-      </c>
-      <c r="O4" s="1">
-        <v>6</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V4" s="1">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>999064416816</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1850</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>17</v>
-      </c>
-      <c r="N5" s="1">
-        <v>20</v>
-      </c>
-      <c r="O5" s="1">
-        <v>6</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" s="1">
-        <v>0</v>
-      </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1">
-        <f t="shared" ref="U5:U8" si="4">VLOOKUP(E5,T_OPERADORES,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="V5" s="1">
-        <f t="shared" ref="V5:V8" si="5">VLOOKUP(G5,T_TIPO_ENVIO,2,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>999064418709</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1854</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
-      <c r="M6" s="1">
-        <v>17</v>
-      </c>
-      <c r="N6" s="1">
-        <v>20</v>
-      </c>
-      <c r="O6" s="1">
-        <v>6</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" s="1">
-        <v>0</v>
-      </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V6" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>999064418842</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1853</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1">
-        <v>17</v>
-      </c>
-      <c r="N7" s="1">
-        <v>20</v>
-      </c>
-      <c r="O7" s="1">
-        <v>6</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S7" s="1">
-        <v>0</v>
-      </c>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V7" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>999064417280</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1848</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
-      <c r="M8" s="1">
-        <v>17</v>
-      </c>
-      <c r="N8" s="1">
-        <v>20</v>
-      </c>
-      <c r="O8" s="1">
-        <v>6</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S8" s="1">
-        <v>0</v>
-      </c>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="V3" si="3">VLOOKUP(G3,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="5" priority="80"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="187"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="188"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="190"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="191"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="200"/>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="duplicateValues" dxfId="3" priority="210"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="0" priority="208"/>
+  <conditionalFormatting sqref="C3:C1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="220"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="1" priority="222"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1413,7 +1116,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,141 +1129,57 @@
       <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>999064414037</v>
-      </c>
-      <c r="B2">
-        <v>4286732494</v>
+      <c r="A2" s="8"/>
+      <c r="B2" t="s">
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>999064416669</v>
-      </c>
-      <c r="B3">
-        <v>1852</v>
-      </c>
+      <c r="A3" s="8"/>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>999064416755</v>
-      </c>
-      <c r="B4">
-        <v>1851</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A4" s="8"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>999064416816</v>
-      </c>
-      <c r="B5">
-        <v>1850</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="8"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>999064418709</v>
-      </c>
-      <c r="B6">
-        <v>1854</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="8"/>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>999064418842</v>
-      </c>
-      <c r="B7">
-        <v>1853</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
+      <c r="A7" s="8"/>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>999064417280</v>
-      </c>
-      <c r="B8">
-        <v>1848</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="8"/>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
correccion de error en el focus de alistamiento
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNOLOGIA-LOGI\Documents\LANCH ALISTAMIENTO FEB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -26,7 +31,7 @@
     <author>Andres</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -42,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="1">
+    <comment ref="K1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1">
+    <comment ref="P1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1">
+    <comment ref="Q1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="58">
   <si>
     <t>Guia</t>
   </si>
@@ -226,7 +231,37 @@
     <t>INTERRAPIDISIMO</t>
   </si>
   <si>
-    <t>ASSG0002</t>
+    <t>FXXI0021</t>
+  </si>
+  <si>
+    <t>XDSG0020</t>
+  </si>
+  <si>
+    <t>XDXI0017</t>
+  </si>
+  <si>
+    <t>FUAP0013</t>
+  </si>
+  <si>
+    <t>DWSG0011</t>
+  </si>
+  <si>
+    <t>XDSG0026</t>
+  </si>
+  <si>
+    <t>062CS24470</t>
+  </si>
+  <si>
+    <t>ACS01847</t>
+  </si>
+  <si>
+    <t>FUSG0059</t>
+  </si>
+  <si>
+    <t>FUSG0038</t>
+  </si>
+  <si>
+    <t>FUSG0057</t>
   </si>
   <si>
     <t>FUSG0010</t>
@@ -235,103 +270,40 @@
     <t>ESSG0009</t>
   </si>
   <si>
-    <t>EP-DG950CBE-BULK</t>
-  </si>
-  <si>
-    <t>XDXI0017</t>
-  </si>
-  <si>
-    <t>XDXI0005</t>
-  </si>
-  <si>
-    <t>DWXI0001</t>
-  </si>
-  <si>
-    <t>FSAP0005</t>
-  </si>
-  <si>
-    <t>FUSG0049</t>
+    <t>ASD02169</t>
+  </si>
+  <si>
+    <t>FUSG0030</t>
+  </si>
+  <si>
+    <t>DWSG0005</t>
   </si>
   <si>
     <t>ASD00540</t>
   </si>
   <si>
-    <t>FXHW0016</t>
-  </si>
-  <si>
-    <t>FXXI0021</t>
-  </si>
-  <si>
-    <t>FXXI0027</t>
-  </si>
-  <si>
-    <t>ACS01721</t>
-  </si>
-  <si>
-    <t>FUAP0006</t>
-  </si>
-  <si>
-    <t>FXXI0022</t>
-  </si>
-  <si>
-    <t>FUSG0050</t>
-  </si>
-  <si>
-    <t>AGL01467</t>
-  </si>
-  <si>
-    <t>XMAP0006</t>
-  </si>
-  <si>
-    <t>ACS01591</t>
-  </si>
-  <si>
-    <t>ESXI0006</t>
-  </si>
-  <si>
-    <t>ASD00261</t>
-  </si>
-  <si>
-    <t>XDXI0011</t>
-  </si>
-  <si>
-    <t>XDXI0007</t>
-  </si>
-  <si>
-    <t>FXHW0007</t>
-  </si>
-  <si>
-    <t>ACEC0021</t>
-  </si>
-  <si>
-    <t>FXXI0010</t>
-  </si>
-  <si>
-    <t>RWSP038</t>
-  </si>
-  <si>
-    <t>GLAP0002</t>
-  </si>
-  <si>
-    <t>054CS22203</t>
-  </si>
-  <si>
-    <t>ADSG0027</t>
-  </si>
-  <si>
-    <t>ACEC0013</t>
-  </si>
-  <si>
-    <t>XDSG0023</t>
-  </si>
-  <si>
-    <t>XDSG0036</t>
+    <t>FXHW0005</t>
+  </si>
+  <si>
+    <t>OU90-BLANCO</t>
+  </si>
+  <si>
+    <t>FUAP0015</t>
+  </si>
+  <si>
+    <t>ADSG0022</t>
+  </si>
+  <si>
+    <t>AGL01511</t>
+  </si>
+  <si>
+    <t>XDXI0018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -484,7 +456,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -567,26 +539,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -607,91 +559,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -811,7 +683,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -846,7 +718,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1055,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V43"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1064,8 +936,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
@@ -1154,13 +1025,13 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <v>40391359307</v>
+        <v>40406627099</v>
       </c>
       <c r="B2" s="1">
-        <v>4354680388</v>
+        <v>4371993842</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1214,15 +1085,15 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <v>40391258260</v>
+        <v>40406614153</v>
       </c>
       <c r="B3" s="1">
-        <v>4354559570</v>
+        <v>4371984097</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1259,7 +1130,7 @@
         <v>33</v>
       </c>
       <c r="S3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1">
@@ -1273,13 +1144,13 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>40391121462</v>
+        <v>40405947212</v>
       </c>
       <c r="B4" s="1">
-        <v>4354403273</v>
+        <v>4371214834</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1318,7 +1189,7 @@
         <v>33</v>
       </c>
       <c r="S4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1">
@@ -1331,14 +1202,14 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>40391082975</v>
+      <c r="A5" s="1">
+        <v>40405603097</v>
       </c>
       <c r="B5" s="1">
-        <v>4354358325</v>
+        <v>4370835271</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1377,7 +1248,7 @@
         <v>33</v>
       </c>
       <c r="S5" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1">
@@ -1390,14 +1261,14 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>40390992647</v>
+      <c r="A6" s="1">
+        <v>40405303907</v>
       </c>
       <c r="B6" s="1">
-        <v>4354249884</v>
+        <v>4370497863</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1436,27 +1307,27 @@
         <v>33</v>
       </c>
       <c r="S6" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1">
-        <f t="shared" ref="U6:U43" si="4">VLOOKUP(E6,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" ref="U6:U28" si="4">VLOOKUP(E6,T_OPERADORES,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="V6" s="1">
-        <f t="shared" ref="V6:V43" si="5">VLOOKUP(G6,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="V6:V28" si="5">VLOOKUP(G6,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>40390992647</v>
+      <c r="A7" s="1">
+        <v>14106660425</v>
       </c>
       <c r="B7" s="1">
-        <v>4354249884</v>
+        <v>4371794940</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -1495,7 +1366,7 @@
         <v>33</v>
       </c>
       <c r="S7" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T7" s="1"/>
       <c r="U7" s="1">
@@ -1508,14 +1379,14 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>40390772978</v>
+      <c r="A8" s="1">
+        <v>40407094766</v>
       </c>
       <c r="B8" s="1">
-        <v>4354005153</v>
+        <v>4372509836</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1554,7 +1425,7 @@
         <v>33</v>
       </c>
       <c r="S8" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="1">
@@ -1568,13 +1439,13 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>40390322135</v>
+        <v>14106655672</v>
       </c>
       <c r="B9" s="1">
-        <v>4353487232</v>
+        <v>4372388333</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1613,7 +1484,7 @@
         <v>33</v>
       </c>
       <c r="S9" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1">
@@ -1627,13 +1498,13 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>40389811922</v>
+        <v>14106654957</v>
       </c>
       <c r="B10" s="1">
-        <v>4352906270</v>
+        <v>4372343677</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1672,7 +1543,7 @@
         <v>33</v>
       </c>
       <c r="S10" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T10" s="1"/>
       <c r="U10" s="1">
@@ -1686,16 +1557,16 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>40389204782</v>
+        <v>14106654957</v>
       </c>
       <c r="B11" s="1">
-        <v>4352212513</v>
+        <v>4372343677</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>32</v>
@@ -1731,7 +1602,7 @@
         <v>33</v>
       </c>
       <c r="S11" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="1">
@@ -1745,13 +1616,13 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>14106471382</v>
+        <v>14106654957</v>
       </c>
       <c r="B12" s="1">
-        <v>4355535617</v>
+        <v>4372343677</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -1790,7 +1661,7 @@
         <v>33</v>
       </c>
       <c r="S12" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="T12" s="1"/>
       <c r="U12" s="1">
@@ -1804,13 +1675,13 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>14106471115</v>
+        <v>40403052893</v>
       </c>
       <c r="B13" s="1">
-        <v>4352833952</v>
+        <v>4367960565</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1849,7 +1720,7 @@
         <v>33</v>
       </c>
       <c r="S13" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="1">
@@ -1863,13 +1734,13 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>14106470530</v>
+        <v>40406892719</v>
       </c>
       <c r="B14" s="1">
-        <v>4355503070</v>
+        <v>4372287299</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1908,7 +1779,7 @@
         <v>33</v>
       </c>
       <c r="S14" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="T14" s="1"/>
       <c r="U14" s="1">
@@ -1922,13 +1793,13 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>40391688319</v>
+        <v>40406832490</v>
       </c>
       <c r="B15" s="1">
-        <v>4355048674</v>
+        <v>4372218803</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1967,7 +1838,7 @@
         <v>33</v>
       </c>
       <c r="S15" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="T15" s="1"/>
       <c r="U15" s="1">
@@ -1981,13 +1852,13 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14106458523</v>
+        <v>14106650800</v>
       </c>
       <c r="B16" s="1">
-        <v>4342656887</v>
+        <v>4371943259</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -2026,7 +1897,7 @@
         <v>33</v>
       </c>
       <c r="S16" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="T16" s="1"/>
       <c r="U16" s="1">
@@ -2040,10 +1911,10 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>14106457453</v>
+        <v>14106650188</v>
       </c>
       <c r="B17" s="1">
-        <v>4354779867</v>
+        <v>4371863630</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>50</v>
@@ -2085,7 +1956,7 @@
         <v>33</v>
       </c>
       <c r="S17" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T17" s="1"/>
       <c r="U17" s="1">
@@ -2099,13 +1970,13 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>14106457453</v>
+        <v>14106649586</v>
       </c>
       <c r="B18" s="1">
-        <v>4354779867</v>
+        <v>4371799725</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -2144,7 +2015,7 @@
         <v>33</v>
       </c>
       <c r="S18" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="T18" s="1"/>
       <c r="U18" s="1">
@@ -2158,13 +2029,13 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>14106457427</v>
+        <v>40406330393</v>
       </c>
       <c r="B19" s="1">
-        <v>4354766718</v>
+        <v>4371652226</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -2203,7 +2074,7 @@
         <v>33</v>
       </c>
       <c r="S19" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="1">
@@ -2217,13 +2088,13 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>14106457329</v>
+        <v>40405515905</v>
       </c>
       <c r="B20" s="1">
-        <v>4354751361</v>
+        <v>4370737186</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -2262,7 +2133,7 @@
         <v>33</v>
       </c>
       <c r="S20" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="T20" s="1"/>
       <c r="U20" s="1">
@@ -2276,13 +2147,13 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>14106456666</v>
+        <v>14106645864</v>
       </c>
       <c r="B21" s="1">
-        <v>4354685469</v>
+        <v>4371199276</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -2321,7 +2192,7 @@
         <v>33</v>
       </c>
       <c r="S21" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="T21" s="1"/>
       <c r="U21" s="1">
@@ -2335,13 +2206,13 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>40391033054</v>
+        <v>14106643569</v>
       </c>
       <c r="B22" s="1">
-        <v>4354300502</v>
+        <v>4370974479</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -2380,7 +2251,7 @@
         <v>33</v>
       </c>
       <c r="S22" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1">
@@ -2394,13 +2265,13 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>14106454790</v>
+        <v>14106643544</v>
       </c>
       <c r="B23" s="1">
-        <v>4354266405</v>
+        <v>4371060573</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -2439,7 +2310,7 @@
         <v>33</v>
       </c>
       <c r="S23" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="1">
@@ -2453,13 +2324,13 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>14106454532</v>
+        <v>14106643266</v>
       </c>
       <c r="B24" s="1">
-        <v>4354179972</v>
+        <v>4371040228</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -2498,7 +2369,7 @@
         <v>33</v>
       </c>
       <c r="S24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="T24" s="1"/>
       <c r="U24" s="1">
@@ -2512,13 +2383,13 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>40390786757</v>
+        <v>14106643171</v>
       </c>
       <c r="B25" s="1">
-        <v>4354016867</v>
+        <v>4370713412</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -2557,7 +2428,7 @@
         <v>33</v>
       </c>
       <c r="S25" s="1">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="1">
@@ -2571,13 +2442,13 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>14106453332</v>
+        <v>40402315377</v>
       </c>
       <c r="B26" s="1">
-        <v>4353851128</v>
+        <v>4367120178</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -2616,7 +2487,7 @@
         <v>33</v>
       </c>
       <c r="S26" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="T26" s="1"/>
       <c r="U26" s="1">
@@ -2630,13 +2501,13 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>14106451079</v>
+        <v>14106641344</v>
       </c>
       <c r="B27" s="1">
-        <v>4353333274</v>
+        <v>4370907968</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
@@ -2675,7 +2546,7 @@
         <v>33</v>
       </c>
       <c r="S27" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="T27" s="1"/>
       <c r="U27" s="1">
@@ -2689,13 +2560,13 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>40390184874</v>
+        <v>14106587871</v>
       </c>
       <c r="B28" s="1">
-        <v>4353332251</v>
+        <v>4365579442</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -2734,7 +2605,7 @@
         <v>33</v>
       </c>
       <c r="S28" s="1">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="T28" s="1"/>
       <c r="U28" s="1">
@@ -2746,971 +2617,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>14106451032</v>
-      </c>
-      <c r="B29" s="1">
-        <v>4352818850</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="1">
-        <v>0</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K29" s="1">
-        <v>1</v>
-      </c>
-      <c r="L29" s="1">
-        <v>1</v>
-      </c>
-      <c r="M29" s="1">
-        <v>17</v>
-      </c>
-      <c r="N29" s="1">
-        <v>20</v>
-      </c>
-      <c r="O29" s="1">
-        <v>6</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S29" s="1">
-        <v>27</v>
-      </c>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V29" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>40389800678</v>
-      </c>
-      <c r="B30" s="1">
-        <v>4352892686</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K30" s="1">
-        <v>1</v>
-      </c>
-      <c r="L30" s="1">
-        <v>1</v>
-      </c>
-      <c r="M30" s="1">
-        <v>17</v>
-      </c>
-      <c r="N30" s="1">
-        <v>20</v>
-      </c>
-      <c r="O30" s="1">
-        <v>6</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S30" s="1">
-        <v>28</v>
-      </c>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V30" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>40389300787</v>
-      </c>
-      <c r="B31" s="1">
-        <v>4352322099</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K31" s="1">
-        <v>1</v>
-      </c>
-      <c r="L31" s="1">
-        <v>1</v>
-      </c>
-      <c r="M31" s="1">
-        <v>17</v>
-      </c>
-      <c r="N31" s="1">
-        <v>20</v>
-      </c>
-      <c r="O31" s="1">
-        <v>6</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S31" s="1">
-        <v>29</v>
-      </c>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V31" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>40389267456</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4352282299</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K32" s="1">
-        <v>1</v>
-      </c>
-      <c r="L32" s="1">
-        <v>1</v>
-      </c>
-      <c r="M32" s="1">
-        <v>17</v>
-      </c>
-      <c r="N32" s="1">
-        <v>20</v>
-      </c>
-      <c r="O32" s="1">
-        <v>6</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S32" s="1">
-        <v>30</v>
-      </c>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V32" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>40389267456</v>
-      </c>
-      <c r="B33" s="1">
-        <v>4352282299</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K33" s="1">
-        <v>1</v>
-      </c>
-      <c r="L33" s="1">
-        <v>1</v>
-      </c>
-      <c r="M33" s="1">
-        <v>17</v>
-      </c>
-      <c r="N33" s="1">
-        <v>20</v>
-      </c>
-      <c r="O33" s="1">
-        <v>6</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S33" s="1">
-        <v>31</v>
-      </c>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V33" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>14106440495</v>
-      </c>
-      <c r="B34" s="1">
-        <v>4351643676</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K34" s="1">
-        <v>1</v>
-      </c>
-      <c r="L34" s="1">
-        <v>1</v>
-      </c>
-      <c r="M34" s="1">
-        <v>17</v>
-      </c>
-      <c r="N34" s="1">
-        <v>20</v>
-      </c>
-      <c r="O34" s="1">
-        <v>6</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S34" s="1">
-        <v>32</v>
-      </c>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V34" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>14106437120</v>
-      </c>
-      <c r="B35" s="1">
-        <v>4351304058</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="1">
-        <v>0</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K35" s="1">
-        <v>1</v>
-      </c>
-      <c r="L35" s="1">
-        <v>1</v>
-      </c>
-      <c r="M35" s="1">
-        <v>17</v>
-      </c>
-      <c r="N35" s="1">
-        <v>20</v>
-      </c>
-      <c r="O35" s="1">
-        <v>6</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S35" s="1">
-        <v>33</v>
-      </c>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V35" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>40384488032</v>
-      </c>
-      <c r="B36" s="1">
-        <v>4346870025</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K36" s="1">
-        <v>1</v>
-      </c>
-      <c r="L36" s="1">
-        <v>1</v>
-      </c>
-      <c r="M36" s="1">
-        <v>17</v>
-      </c>
-      <c r="N36" s="1">
-        <v>20</v>
-      </c>
-      <c r="O36" s="1">
-        <v>6</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S36" s="1">
-        <v>34</v>
-      </c>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V36" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>40388220305</v>
-      </c>
-      <c r="B37" s="1">
-        <v>4351091038</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F37" s="1">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K37" s="1">
-        <v>1</v>
-      </c>
-      <c r="L37" s="1">
-        <v>1</v>
-      </c>
-      <c r="M37" s="1">
-        <v>17</v>
-      </c>
-      <c r="N37" s="1">
-        <v>20</v>
-      </c>
-      <c r="O37" s="1">
-        <v>6</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S37" s="1">
-        <v>35</v>
-      </c>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V37" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>40388220305</v>
-      </c>
-      <c r="B38" s="1">
-        <v>4351091038</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F38" s="1">
-        <v>0</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K38" s="1">
-        <v>1</v>
-      </c>
-      <c r="L38" s="1">
-        <v>1</v>
-      </c>
-      <c r="M38" s="1">
-        <v>17</v>
-      </c>
-      <c r="N38" s="1">
-        <v>20</v>
-      </c>
-      <c r="O38" s="1">
-        <v>6</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S38" s="1">
-        <v>36</v>
-      </c>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V38" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>14106434293</v>
-      </c>
-      <c r="B39" s="1">
-        <v>4350949181</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" s="1">
-        <v>0</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K39" s="1">
-        <v>1</v>
-      </c>
-      <c r="L39" s="1">
-        <v>1</v>
-      </c>
-      <c r="M39" s="1">
-        <v>17</v>
-      </c>
-      <c r="N39" s="1">
-        <v>20</v>
-      </c>
-      <c r="O39" s="1">
-        <v>6</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S39" s="1">
-        <v>37</v>
-      </c>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V39" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>40387813877</v>
-      </c>
-      <c r="B40" s="1">
-        <v>4350632475</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F40" s="1">
-        <v>0</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K40" s="1">
-        <v>1</v>
-      </c>
-      <c r="L40" s="1">
-        <v>1</v>
-      </c>
-      <c r="M40" s="1">
-        <v>17</v>
-      </c>
-      <c r="N40" s="1">
-        <v>20</v>
-      </c>
-      <c r="O40" s="1">
-        <v>6</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S40" s="1">
-        <v>38</v>
-      </c>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V40" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>14106430912</v>
-      </c>
-      <c r="B41" s="1">
-        <v>4349017581</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F41" s="1">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K41" s="1">
-        <v>1</v>
-      </c>
-      <c r="L41" s="1">
-        <v>1</v>
-      </c>
-      <c r="M41" s="1">
-        <v>17</v>
-      </c>
-      <c r="N41" s="1">
-        <v>20</v>
-      </c>
-      <c r="O41" s="1">
-        <v>6</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S41" s="1">
-        <v>39</v>
-      </c>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V41" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>14106430692</v>
-      </c>
-      <c r="B42" s="1">
-        <v>4350596001</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F42" s="1">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K42" s="1">
-        <v>1</v>
-      </c>
-      <c r="L42" s="1">
-        <v>1</v>
-      </c>
-      <c r="M42" s="1">
-        <v>17</v>
-      </c>
-      <c r="N42" s="1">
-        <v>20</v>
-      </c>
-      <c r="O42" s="1">
-        <v>6</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S42" s="1">
-        <v>40</v>
-      </c>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V42" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>14106427532</v>
-      </c>
-      <c r="B43" s="1">
-        <v>4350468607</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" s="1">
-        <v>0</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="1">
-        <v>1</v>
-      </c>
-      <c r="L43" s="1">
-        <v>1</v>
-      </c>
-      <c r="M43" s="1">
-        <v>17</v>
-      </c>
-      <c r="N43" s="1">
-        <v>20</v>
-      </c>
-      <c r="O43" s="1">
-        <v>6</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S43" s="1">
-        <v>41</v>
-      </c>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="V43" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="26" priority="143"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="185"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="25" priority="237"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="279"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C1048576">
-    <cfRule type="duplicateValues" dxfId="24" priority="247"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="289"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="23" priority="249"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="57"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="12" priority="58"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="11" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="10" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="22" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="21" priority="26"/>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="8" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="20" priority="27"/>
+  <conditionalFormatting sqref="A1:A2 A4:A10 A13:A1048576">
+    <cfRule type="duplicateValues" dxfId="7" priority="379"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A6 A8:A17 A19:A32 A34:A37 A39:A1048576">
-    <cfRule type="duplicateValues" dxfId="19" priority="18"/>
+  <conditionalFormatting sqref="B1 B4:B10 B13:B1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="383"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B6 B8:B17 B19:B32 B34:B37 B39:B1048576">
-    <cfRule type="duplicateValues" dxfId="18" priority="17"/>
+  <conditionalFormatting sqref="A1:A2 A4:A10 A13:A1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="387"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2 A4:A6 A8:A17 A19:A32 A34:A37 A39:A1048576">
-    <cfRule type="duplicateValues" dxfId="17" priority="253"/>
+  <conditionalFormatting sqref="B1 B4:B10 B13:B1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="391"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B2 B4:B6 B8:B17 B19:B32 B34:B37 B39:B1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="257"/>
+  <conditionalFormatting sqref="A11:A12">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
+  <conditionalFormatting sqref="B11:B12">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="12" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
+  <conditionalFormatting sqref="A11:A12">
     <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
+  <conditionalFormatting sqref="B11:B12">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3823,10 +2779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3840,13 +2796,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <v>40391359307</v>
+        <v>40406627099</v>
       </c>
       <c r="B2">
-        <v>4354680388</v>
+        <v>4371993842</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3854,19 +2810,17 @@
       <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <v>40391258260</v>
+        <v>40406614153</v>
       </c>
       <c r="B3">
-        <v>4354559570</v>
+        <v>4371984097</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3874,74 +2828,71 @@
       <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>40391121462</v>
+        <v>40405947212</v>
       </c>
       <c r="B4">
-        <v>4354403273</v>
+        <v>4371214834</v>
       </c>
       <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40405603097</v>
+      </c>
+      <c r="B5">
+        <v>4370835271</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>40405303907</v>
+      </c>
+      <c r="B6">
+        <v>4370497863</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>40391082975</v>
-      </c>
-      <c r="B5">
-        <v>4354358325</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>40390992647</v>
-      </c>
-      <c r="B6">
-        <v>4354249884</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7">
+        <v>14106660425</v>
+      </c>
+      <c r="B7">
+        <v>4371794940</v>
+      </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3949,19 +2900,17 @@
       <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>40390772978</v>
+      <c r="A8">
+        <v>40407094766</v>
       </c>
       <c r="B8">
-        <v>4354005153</v>
+        <v>4372509836</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3969,19 +2918,17 @@
       <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40390322135</v>
+        <v>14106655672</v>
       </c>
       <c r="B9">
-        <v>4353487232</v>
+        <v>4372388333</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3989,19 +2936,17 @@
       <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40389811922</v>
+        <v>14106654957</v>
       </c>
       <c r="B10">
-        <v>4352906270</v>
+        <v>4372343677</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -4009,19 +2954,11 @@
       <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>40389204782</v>
-      </c>
-      <c r="B11">
-        <v>4352212513</v>
-      </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -4029,19 +2966,11 @@
       <c r="E11" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>14106471382</v>
-      </c>
-      <c r="B12">
-        <v>4355535617</v>
-      </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -4049,19 +2978,11 @@
       <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>14106471115</v>
-      </c>
-      <c r="B13">
-        <v>4352833952</v>
-      </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -4069,19 +2990,17 @@
       <c r="E13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14106470530</v>
+        <v>40403052893</v>
       </c>
       <c r="B14">
-        <v>4355503070</v>
+        <v>4367960565</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -4089,19 +3008,17 @@
       <c r="E14" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>40391688319</v>
+        <v>40406892719</v>
       </c>
       <c r="B15">
-        <v>4355048674</v>
+        <v>4372287299</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -4109,19 +3026,17 @@
       <c r="E15" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14106458523</v>
+        <v>40406832490</v>
       </c>
       <c r="B16">
-        <v>4342656887</v>
+        <v>4372218803</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -4129,53 +3044,53 @@
       <c r="E16" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>14106457453</v>
+        <v>14106650800</v>
       </c>
       <c r="B17">
-        <v>4354779867</v>
+        <v>4371943259</v>
       </c>
       <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14106650188</v>
+      </c>
+      <c r="B18">
+        <v>4371863630</v>
+      </c>
+      <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>14106457427</v>
+        <v>14106649586</v>
       </c>
       <c r="B19">
-        <v>4354766718</v>
+        <v>4371799725</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -4183,19 +3098,17 @@
       <c r="E19" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>14106457329</v>
+        <v>40406330393</v>
       </c>
       <c r="B20">
-        <v>4354751361</v>
+        <v>4371652226</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -4203,19 +3116,17 @@
       <c r="E20" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>14106456666</v>
+        <v>40405515905</v>
       </c>
       <c r="B21">
-        <v>4354685469</v>
+        <v>4370737186</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -4223,19 +3134,17 @@
       <c r="E21" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>40391033054</v>
+        <v>14106645864</v>
       </c>
       <c r="B22">
-        <v>4354300502</v>
+        <v>4371199276</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -4243,19 +3152,17 @@
       <c r="E22" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>14106454790</v>
+        <v>14106643569</v>
       </c>
       <c r="B23">
-        <v>4354266405</v>
+        <v>4370974479</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -4263,19 +3170,17 @@
       <c r="E23" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>14106454532</v>
+        <v>14106643544</v>
       </c>
       <c r="B24">
-        <v>4354179972</v>
+        <v>4371060573</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -4283,19 +3188,17 @@
       <c r="E24" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>40390786757</v>
+        <v>14106643266</v>
       </c>
       <c r="B25">
-        <v>4354016867</v>
+        <v>4371040228</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -4303,19 +3206,17 @@
       <c r="E25" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>14106453332</v>
+        <v>14106643171</v>
       </c>
       <c r="B26">
-        <v>4353851128</v>
+        <v>4370713412</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -4323,19 +3224,17 @@
       <c r="E26" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>14106451079</v>
+        <v>40402315377</v>
       </c>
       <c r="B27">
-        <v>4353333274</v>
+        <v>4367120178</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -4343,19 +3242,17 @@
       <c r="E27" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>40390184874</v>
+        <v>14106641344</v>
       </c>
       <c r="B28">
-        <v>4353332251</v>
+        <v>4370907968</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -4363,19 +3260,17 @@
       <c r="E28" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>14106451032</v>
+        <v>14106587871</v>
       </c>
       <c r="B29">
-        <v>4352818850</v>
+        <v>4365579442</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -4383,277 +3278,37 @@
       <c r="E29" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>40389800678</v>
-      </c>
-      <c r="B30">
-        <v>4352892686</v>
-      </c>
-      <c r="C30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>40389300787</v>
-      </c>
-      <c r="B31">
-        <v>4352322099</v>
-      </c>
-      <c r="C31" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>40389267456</v>
-      </c>
-      <c r="B32">
-        <v>4352282299</v>
-      </c>
-      <c r="C32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>14106440495</v>
-      </c>
-      <c r="B34">
-        <v>4351643676</v>
-      </c>
-      <c r="C34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>14106437120</v>
-      </c>
-      <c r="B35">
-        <v>4351304058</v>
-      </c>
-      <c r="C35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>40384488032</v>
-      </c>
-      <c r="B36">
-        <v>4346870025</v>
-      </c>
-      <c r="C36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>40388220305</v>
-      </c>
-      <c r="B37">
-        <v>4351091038</v>
-      </c>
-      <c r="C37" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>32</v>
-      </c>
-      <c r="F37" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>32</v>
-      </c>
-      <c r="F38" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>14106434293</v>
-      </c>
-      <c r="B39">
-        <v>4350949181</v>
-      </c>
-      <c r="C39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>40387813877</v>
-      </c>
-      <c r="B40">
-        <v>4350632475</v>
-      </c>
-      <c r="C40" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F40" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>14106430912</v>
-      </c>
-      <c r="B41">
-        <v>4349017581</v>
-      </c>
-      <c r="C41" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F41" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>14106430692</v>
-      </c>
-      <c r="B42">
-        <v>4350596001</v>
-      </c>
-      <c r="C42" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F42" s="7">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>14106427532</v>
-      </c>
-      <c r="B43">
-        <v>4350468607</v>
-      </c>
-      <c r="C43" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" s="7">
-        <v>44235</v>
-      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correccion de error en fecha de actualizacion de salidas producto
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="56">
   <si>
     <t>Guia</t>
   </si>
@@ -162,9 +162,6 @@
     <t>OPERADORES</t>
   </si>
   <si>
-    <t>INTERAPIDISIMO</t>
-  </si>
-  <si>
     <t>TIPO ENVIO</t>
   </si>
   <si>
@@ -231,118 +228,70 @@
     <t>ACCESORIOS CELULAR</t>
   </si>
   <si>
-    <t>MASLOGISTICA - FLEX</t>
-  </si>
-  <si>
-    <t>AGL01467</t>
-  </si>
-  <si>
-    <t>Felipe Campos</t>
-  </si>
-  <si>
-    <t>Kr 79 #128-95 / Unidad 6 int 3 Apto 601 - Balcones de lindaraja, Usaquén, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>Mariana Agudelo G</t>
-  </si>
-  <si>
-    <t>Carrera 5 #86-05 / Apt 303 - Refugio, Usaquén, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>000GL21813</t>
-  </si>
-  <si>
-    <t>ACS02159</t>
-  </si>
-  <si>
-    <t>Sebastián Ríos</t>
-  </si>
-  <si>
-    <t>Calle 7A BIS C #80A- 50 / APTO 508D - Kennedy, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>AGL02243</t>
-  </si>
-  <si>
-    <t>EF-ZN980CBEGUS</t>
-  </si>
-  <si>
-    <t>malcom robinson</t>
-  </si>
-  <si>
-    <t>Calle 35 #15-32 / Oficina Cultural Embajada De Italia - Teusaquillo, Teusaquillo, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>XDAP0017</t>
-  </si>
-  <si>
-    <t>PRO NUTRITION</t>
-  </si>
-  <si>
-    <t>CALLE 2 A #42-05 / Jazmin, Puente Aranda, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>076CS27179</t>
-  </si>
-  <si>
-    <t>Felipe Lopez</t>
-  </si>
-  <si>
-    <t>Carrera 10bis #22-42 / Sur - Sociego, Rafael Uribe Uribe, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>042GL20423</t>
-  </si>
-  <si>
-    <t>FUSG0029</t>
-  </si>
-  <si>
-    <t>Ricardo Criales Zopoaragon</t>
-  </si>
-  <si>
-    <t>Av. Carrera 9 #146 -45 / Apto 713 - Cedritos, Usaquén, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>ASD01117</t>
-  </si>
-  <si>
-    <t>Jenny García</t>
-  </si>
-  <si>
-    <t>Carrera 50 #124-46 / Apto 204 Edificio Baluarte - El batan, Suba, Bogotá D.C.</t>
+    <t>INTERRAPIDISIMO</t>
+  </si>
+  <si>
+    <t>EP-TA20JBEUGUS</t>
+  </si>
+  <si>
+    <t>ACS00428</t>
+  </si>
+  <si>
+    <t>EP-TA50JBE-BULK</t>
+  </si>
+  <si>
+    <t>FXXI0010</t>
+  </si>
+  <si>
+    <t>064GL24527</t>
+  </si>
+  <si>
+    <t>XDSG0036</t>
+  </si>
+  <si>
+    <t>FUSG0062</t>
+  </si>
+  <si>
+    <t>DWHW0004</t>
+  </si>
+  <si>
+    <t>DWXI0001</t>
+  </si>
+  <si>
+    <t>FXXI0013</t>
+  </si>
+  <si>
+    <t>XDAP0003</t>
+  </si>
+  <si>
+    <t>ACRI0007</t>
+  </si>
+  <si>
+    <t>DWSG0011</t>
+  </si>
+  <si>
+    <t>FXXI0027</t>
+  </si>
+  <si>
+    <t>DWXI0003</t>
   </si>
   <si>
     <t>EP-DG950CBE-BULK</t>
   </si>
   <si>
-    <t>Diego Moscoso</t>
-  </si>
-  <si>
-    <t>Calle 164 #19-15 / Torre 1 Apartamento 303 - Orquideas, Usaquén, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>luis alejandro aragon</t>
-  </si>
-  <si>
-    <t>Calle 23a Bis #85a-25 / Ed Balmoral 1, apto 607 - modelia, Fontibón, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>FXHW0014</t>
-  </si>
-  <si>
-    <t>Carlos Maqueo B</t>
-  </si>
-  <si>
-    <t>Carrera 82 #17-95 / Conjunto Lantana Real Torre 10 apto 702 - Fontibón, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>ESSG0009</t>
-  </si>
-  <si>
-    <t>Daniela Paolini</t>
-  </si>
-  <si>
-    <t>Calle 102A #11B-32 / Apto 202 - Rincon del Chico, Usaquén, Bogotá D.C.</t>
+    <t>ASD00540</t>
+  </si>
+  <si>
+    <t>XDXI0017</t>
+  </si>
+  <si>
+    <t>076CS27184</t>
+  </si>
+  <si>
+    <t>FUAP0007</t>
+  </si>
+  <si>
+    <t>EF-ZN985CBEGUS</t>
   </si>
 </sst>
 </file>
@@ -476,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -493,6 +442,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -500,7 +450,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="25">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -508,16 +458,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -533,11 +473,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -563,11 +503,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -583,11 +523,141 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -931,7 +1001,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -940,15 +1010,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
@@ -977,10 +1046,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>5</v>
@@ -989,76 +1058,69 @@
         <v>6</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="U1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>40419602988</v>
+      <c r="A2" s="8">
+        <v>40425005995</v>
       </c>
       <c r="B2" s="1">
-        <v>4386747582</v>
+        <v>4392898835</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="K2">
         <v>1</v>
       </c>
@@ -1075,20 +1137,20 @@
         <v>6</v>
       </c>
       <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
       <c r="R2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="U2" s="1">
         <f t="shared" ref="U2" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V2" s="1">
         <f t="shared" ref="V2" si="1">VLOOKUP(G2,T_TIPO_ENVIO,2,FALSE)</f>
@@ -1096,35 +1158,26 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>40419602988</v>
+      <c r="A3" s="8">
+        <v>40424250919</v>
       </c>
       <c r="B3" s="1">
-        <v>4386747582</v>
+        <v>4392034316</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K3" s="1">
         <v>1</v>
@@ -1142,56 +1195,48 @@
         <v>6</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S3" s="1">
         <v>0</v>
       </c>
+      <c r="T3" s="1"/>
       <c r="U3" s="1">
-        <f t="shared" ref="U3:U4" si="2">VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
-        <v>4</v>
+        <f t="shared" ref="U3:U5" si="2">VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="V3" s="1">
-        <f t="shared" ref="V3:V4" si="3">VLOOKUP(G3,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="V3:V5" si="3">VLOOKUP(G3,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>40419566212</v>
+      <c r="A4" s="8">
+        <v>40424166959</v>
       </c>
       <c r="B4" s="1">
-        <v>4386709211</v>
+        <v>4391939341</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
@@ -1209,13 +1254,13 @@
         <v>6</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S4" s="1">
         <v>0</v>
@@ -1223,7 +1268,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V4" s="1">
         <f t="shared" si="3"/>
@@ -1231,35 +1276,26 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>40419490081</v>
+      <c r="A5" s="8">
+        <v>40424008430</v>
       </c>
       <c r="B5" s="1">
-        <v>4386622544</v>
+        <v>4391759105</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K5" s="1">
         <v>1</v>
@@ -1277,57 +1313,48 @@
         <v>6</v>
       </c>
       <c r="P5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1">
-        <f t="shared" ref="U5:U14" si="4">VLOOKUP(E5,T_OPERADORES,2,FALSE)</f>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="V5" s="1">
-        <f t="shared" ref="V5:V14" si="5">VLOOKUP(G5,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>40419466006</v>
+      <c r="A6" s="8">
+        <v>40424008430</v>
       </c>
       <c r="B6" s="1">
-        <v>4386595546</v>
+        <v>4391759105</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K6" s="1">
         <v>1</v>
@@ -1345,57 +1372,48 @@
         <v>6</v>
       </c>
       <c r="P6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S6" s="1">
         <v>0</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" ref="U6:U24" si="4">VLOOKUP(E6,T_OPERADORES,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="V6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="V6:V24" si="5">VLOOKUP(G6,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>40419293234</v>
+        <v>14107883757</v>
       </c>
       <c r="B7" s="1">
-        <v>4386399886</v>
+        <v>4393385237</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
@@ -1413,13 +1431,13 @@
         <v>6</v>
       </c>
       <c r="P7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S7" s="1">
         <v>0</v>
@@ -1427,7 +1445,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V7" s="1">
         <f t="shared" si="5"/>
@@ -1436,34 +1454,25 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>40419186243</v>
+        <v>14107882254</v>
       </c>
       <c r="B8" s="1">
-        <v>4386283186</v>
+        <v>4393309790</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K8" s="1">
         <v>1</v>
@@ -1481,13 +1490,13 @@
         <v>6</v>
       </c>
       <c r="P8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S8" s="1">
         <v>0</v>
@@ -1495,7 +1504,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V8" s="1">
         <f t="shared" si="5"/>
@@ -1504,34 +1513,25 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>40418807762</v>
+        <v>14107882254</v>
       </c>
       <c r="B9" s="1">
-        <v>4385849036</v>
+        <v>4393309790</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K9" s="1">
         <v>1</v>
@@ -1549,13 +1549,13 @@
         <v>6</v>
       </c>
       <c r="P9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
@@ -1563,7 +1563,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V9" s="1">
         <f t="shared" si="5"/>
@@ -1572,34 +1572,25 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>40418773872</v>
+        <v>14107877898</v>
       </c>
       <c r="B10" s="1">
-        <v>4385804072</v>
+        <v>4393092109</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K10" s="1">
         <v>1</v>
@@ -1617,13 +1608,13 @@
         <v>6</v>
       </c>
       <c r="P10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
@@ -1631,7 +1622,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V10" s="1">
         <f t="shared" si="5"/>
@@ -1640,34 +1631,25 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>40418504234</v>
+        <v>14107872030</v>
       </c>
       <c r="B11" s="1">
-        <v>4385498310</v>
+        <v>4392459830</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K11" s="1">
         <v>1</v>
@@ -1685,13 +1667,13 @@
         <v>6</v>
       </c>
       <c r="P11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S11" s="1">
         <v>0</v>
@@ -1699,7 +1681,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V11" s="1">
         <f t="shared" si="5"/>
@@ -1708,34 +1690,25 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>40417961365</v>
+        <v>40424611965</v>
       </c>
       <c r="B12" s="1">
-        <v>4384881455</v>
+        <v>4392444112</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K12" s="1">
         <v>1</v>
@@ -1753,13 +1726,13 @@
         <v>6</v>
       </c>
       <c r="P12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S12" s="1">
         <v>0</v>
@@ -1767,7 +1740,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V12" s="1">
         <f t="shared" si="5"/>
@@ -1776,34 +1749,25 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>40417944715</v>
+        <v>14107871401</v>
       </c>
       <c r="B13" s="1">
-        <v>4384863201</v>
+        <v>4392307665</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K13" s="1">
         <v>1</v>
@@ -1821,13 +1785,13 @@
         <v>6</v>
       </c>
       <c r="P13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q13" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S13" s="1">
         <v>0</v>
@@ -1835,7 +1799,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V13" s="1">
         <f t="shared" si="5"/>
@@ -1844,34 +1808,25 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>40417875900</v>
+        <v>14107871401</v>
       </c>
       <c r="B14" s="1">
-        <v>4384784582</v>
+        <v>4392307665</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K14" s="1">
         <v>1</v>
@@ -1889,13 +1844,13 @@
         <v>6</v>
       </c>
       <c r="P14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q14" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S14" s="1">
         <v>0</v>
@@ -1903,52 +1858,678 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V14" s="1">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>40424441539</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4392246511</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1">
+        <v>17</v>
+      </c>
+      <c r="N15" s="1">
+        <v>20</v>
+      </c>
+      <c r="O15" s="1">
+        <v>6</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V15" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>40424376198</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4392177065</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>17</v>
+      </c>
+      <c r="N16" s="1">
+        <v>20</v>
+      </c>
+      <c r="O16" s="1">
+        <v>6</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V16" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>14107870334</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4391662345</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1">
+        <v>17</v>
+      </c>
+      <c r="N17" s="1">
+        <v>20</v>
+      </c>
+      <c r="O17" s="1">
+        <v>6</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V17" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>40424210132</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4391988139</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+      <c r="M18" s="1">
+        <v>17</v>
+      </c>
+      <c r="N18" s="1">
+        <v>20</v>
+      </c>
+      <c r="O18" s="1">
+        <v>6</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V18" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>14107868986</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4391932652</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1">
+        <v>17</v>
+      </c>
+      <c r="N19" s="1">
+        <v>20</v>
+      </c>
+      <c r="O19" s="1">
+        <v>6</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S19" s="1">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V19" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>14107867386</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4391857169</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="M20" s="1">
+        <v>17</v>
+      </c>
+      <c r="N20" s="1">
+        <v>20</v>
+      </c>
+      <c r="O20" s="1">
+        <v>6</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V20" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>40424053314</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4391809262</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1">
+        <v>17</v>
+      </c>
+      <c r="N21" s="1">
+        <v>20</v>
+      </c>
+      <c r="O21" s="1">
+        <v>6</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V21" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>14107864603</v>
+      </c>
+      <c r="B22" s="1">
+        <v>4391700296</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="M22" s="1">
+        <v>17</v>
+      </c>
+      <c r="N22" s="1">
+        <v>20</v>
+      </c>
+      <c r="O22" s="1">
+        <v>6</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V22" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>14107862844</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4391614907</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1">
+        <v>17</v>
+      </c>
+      <c r="N23" s="1">
+        <v>20</v>
+      </c>
+      <c r="O23" s="1">
+        <v>6</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V23" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>14107860940</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4391459639</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1">
+        <v>17</v>
+      </c>
+      <c r="N24" s="1">
+        <v>20</v>
+      </c>
+      <c r="O24" s="1">
+        <v>6</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V24" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="12" priority="189"/>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="24" priority="237"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="224"/>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="duplicateValues" dxfId="23" priority="331"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="309"/>
+  <conditionalFormatting sqref="C3:C1048576">
+    <cfRule type="duplicateValues" dxfId="22" priority="341"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="9" priority="317"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="109"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2 A4:A1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="409"/>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="20" priority="110"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2 A4:A1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="412"/>
+  <conditionalFormatting sqref="A4:A5 A1:A2 A7:A8 A10:A13 A15:A1048576">
+    <cfRule type="duplicateValues" dxfId="19" priority="501"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B2 B4:B1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="415"/>
+  <conditionalFormatting sqref="B4:B5 B1 B7:B8 B10:B13 B15:B1048576">
+    <cfRule type="duplicateValues" dxfId="18" priority="504"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B2 B4:B1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="418"/>
+  <conditionalFormatting sqref="A4:A5 A1:A2 A7:A8 A10:A13 A15:A1048576">
+    <cfRule type="duplicateValues" dxfId="17" priority="507"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B5 B1 B7:B8 B10:B13 B15:B1048576">
+    <cfRule type="duplicateValues" dxfId="16" priority="510"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1961,7 +2542,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,14 +2552,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="D1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1988,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -2002,7 +2583,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -2018,7 +2599,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -2026,7 +2607,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -2034,7 +2615,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -2042,7 +2623,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -2060,342 +2641,464 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I14"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>40419602988</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>40425005995</v>
       </c>
       <c r="B2">
-        <v>4386747582</v>
+        <v>4392898835</v>
       </c>
       <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>40424250919</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4392034316</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>40424166959</v>
+      </c>
+      <c r="B4">
+        <v>4391939341</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>40424008430</v>
+      </c>
+      <c r="B5">
+        <v>4391759105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>14107883757</v>
+      </c>
+      <c r="B7">
+        <v>4393385237</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>14107882254</v>
+      </c>
+      <c r="B8">
+        <v>4393309790</v>
+      </c>
+      <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="I2" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14107877898</v>
+      </c>
+      <c r="B10">
+        <v>4393092109</v>
+      </c>
+      <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="7">
-        <v>44250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>40419566212</v>
-      </c>
-      <c r="B4">
-        <v>4386709211</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>14107872030</v>
+      </c>
+      <c r="B11">
+        <v>4392459830</v>
+      </c>
+      <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>40424611965</v>
+      </c>
+      <c r="B12">
+        <v>4392444112</v>
+      </c>
+      <c r="C12" t="s">
         <v>47</v>
       </c>
-      <c r="I4" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>14107871401</v>
+      </c>
+      <c r="B13">
+        <v>4392307665</v>
+      </c>
+      <c r="C13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>40419490081</v>
-      </c>
-      <c r="B5">
-        <v>4386622544</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>40424441539</v>
+      </c>
+      <c r="B15">
+        <v>4392246511</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>40424376198</v>
+      </c>
+      <c r="B16">
+        <v>4392177065</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14107870334</v>
+      </c>
+      <c r="B17">
+        <v>4391662345</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>40424210132</v>
+      </c>
+      <c r="B18">
+        <v>4391988139</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14107868986</v>
+      </c>
+      <c r="B19">
+        <v>4391932652</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>14107867386</v>
+      </c>
+      <c r="B20">
+        <v>4391857169</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>40424053314</v>
+      </c>
+      <c r="B21">
+        <v>4391809262</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14107864603</v>
+      </c>
+      <c r="B22">
+        <v>4391700296</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>14107862844</v>
+      </c>
+      <c r="B23">
+        <v>4391614907</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>14107860940</v>
+      </c>
+      <c r="B24">
+        <v>4391459639</v>
+      </c>
+      <c r="C24" t="s">
         <v>36</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>40419466006</v>
-      </c>
-      <c r="B6">
-        <v>4386595546</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>40419293234</v>
-      </c>
-      <c r="B7">
-        <v>4386399886</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>40419186243</v>
-      </c>
-      <c r="B8">
-        <v>4386283186</v>
-      </c>
-      <c r="C8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>40418807762</v>
-      </c>
-      <c r="B9">
-        <v>4385849036</v>
-      </c>
-      <c r="C9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>40418773872</v>
-      </c>
-      <c r="B10">
-        <v>4385804072</v>
-      </c>
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>40418504234</v>
-      </c>
-      <c r="B11">
-        <v>4385498310</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H11" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>40417961365</v>
-      </c>
-      <c r="B12">
-        <v>4384881455</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H12" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>40417944715</v>
-      </c>
-      <c r="B13">
-        <v>4384863201</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H13" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>40417875900</v>
-      </c>
-      <c r="B14">
-        <v>4384784582</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="7">
-        <v>44250</v>
-      </c>
-      <c r="H14" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" t="s">
-        <v>72</v>
-      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actualizacion de carga a mensajero con json
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="84">
   <si>
     <t>Guia</t>
   </si>
@@ -234,28 +234,148 @@
     <t>11D</t>
   </si>
   <si>
-    <t>ACS01721</t>
-  </si>
-  <si>
-    <t>Juan Sebastián Quijano Rodríguez</t>
-  </si>
-  <si>
-    <t>Calle 151 # 11-62 APTO 1101 T3</t>
-  </si>
-  <si>
-    <t>316 8654609</t>
-  </si>
-  <si>
-    <t>AGL01511</t>
-  </si>
-  <si>
-    <t>2A</t>
-  </si>
-  <si>
     <t>ACCESORIOS CEL VENTA 1993</t>
   </si>
   <si>
     <t>CORTESIA</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>EP-TA20JBEUGUS</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>EO-IC100BBEGWW</t>
+  </si>
+  <si>
+    <t>FUAP0013</t>
+  </si>
+  <si>
+    <t>7E</t>
+  </si>
+  <si>
+    <t>Jhoan Castellanos</t>
+  </si>
+  <si>
+    <t>Calle 6 C #73-40 / Casa 36 - Las dos avenidas, Kennedy, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>ACS00603</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>Yolvan Madrid</t>
+  </si>
+  <si>
+    <t>Cl. 22j #113a-40 / conjunto atahualpa torre 4 apt 307 - Atahualpa, Fontibón, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>ADSG0010</t>
+  </si>
+  <si>
+    <t>8D</t>
+  </si>
+  <si>
+    <t>jose castro</t>
+  </si>
+  <si>
+    <t>Calle 33 A #21B-35S / Casa - Quiroga, Rafael Uribe Uribe, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>076CS27179</t>
+  </si>
+  <si>
+    <t>juliana baez</t>
+  </si>
+  <si>
+    <t>Calle 96 #17-18 / Apartamento 101 - Chico, Chapinero, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FXXI0021</t>
+  </si>
+  <si>
+    <t>6F</t>
+  </si>
+  <si>
+    <t>danilo ortega sanchez</t>
+  </si>
+  <si>
+    <t>Carrera 70A # 1 - 10-SN / CENTROAMERICAS, Kennedy, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Yeison Rivera</t>
+  </si>
+  <si>
+    <t>Carrera 94 #42 B 59-SN / Piso 3 - Dindalito, Kennedy, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>ACEC0012</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>Manuel Marin</t>
+  </si>
+  <si>
+    <t>Calle 145 #7a-40 / Casa 20 - Belmira, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>milena ruiz</t>
+  </si>
+  <si>
+    <t>calle 185 #49-60 / Casa 80 - mirandela, Suba, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>EP-TA50JBE-BULK</t>
+  </si>
+  <si>
+    <t>11F</t>
+  </si>
+  <si>
+    <t>Lucas Umaña</t>
+  </si>
+  <si>
+    <t>Diagonal 27 #3a-70 / apto 107 - la macarena, Santa Fe, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FUAP0015</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>Sebastian Luna</t>
+  </si>
+  <si>
+    <t>Calle 49h Sur 7a-06 #SN-SN / Es una casa amarilla - Molinos 1, Tunjuelito, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>EF-ZG985CBEGUS</t>
+  </si>
+  <si>
+    <t>Karime David</t>
+  </si>
+  <si>
+    <t>Carrera 9 #52A-20 / Apto. 201 - Marly, Chapinero, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Tata040 Al</t>
+  </si>
+  <si>
+    <t>Carrera 115 #148-40 / Int 15 501 Flores 1 - Cerca Al Cc Imperial, Suba, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FXXI0017</t>
+  </si>
+  <si>
+    <t>FUSG0022</t>
   </si>
 </sst>
 </file>
@@ -413,7 +533,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -446,21 +566,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -511,6 +631,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -854,11 +1004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,34 +1103,34 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1993</v>
+        <v>40460215902</v>
       </c>
       <c r="B2" s="1">
-        <v>1993</v>
+        <v>4433017396</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1004,50 +1154,50 @@
         <v>29</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="U2" s="1">
         <f t="shared" ref="U2" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V2" s="1">
         <f t="shared" ref="V2" si="1">VLOOKUP(G2,T_TIPO_ENVIO,2,FALSE)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1993</v>
+        <v>40460215902</v>
       </c>
       <c r="B3" s="1">
-        <v>1993</v>
+        <v>4433017396</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
       </c>
       <c r="K3" s="1">
         <v>1</v>
@@ -1071,62 +1221,887 @@
         <v>29</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <f t="shared" ref="U3:U4" si="2">VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="V3" s="1">
+        <f t="shared" ref="V3:V4" si="3">VLOOKUP(G3,T_TIPO_ENVIO,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>40460120772</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4432906989</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>17</v>
+      </c>
+      <c r="N4" s="1">
+        <v>20</v>
+      </c>
+      <c r="O4" s="1">
+        <v>6</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="V4" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>40460111549</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4432901099</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>17</v>
+      </c>
+      <c r="N5" s="1">
+        <v>20</v>
+      </c>
+      <c r="O5" s="1">
+        <v>6</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1">
+        <f t="shared" ref="U5:U15" si="4">VLOOKUP(E5,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="V5" s="1">
+        <f t="shared" ref="V5:V15" si="5">VLOOKUP(G5,T_TIPO_ENVIO,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>40459881021</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4432634573</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>17</v>
+      </c>
+      <c r="N6" s="1">
+        <v>20</v>
+      </c>
+      <c r="O6" s="1">
+        <v>6</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V6" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>40459825586</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4432573874</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
+        <v>17</v>
+      </c>
+      <c r="N7" s="1">
+        <v>20</v>
+      </c>
+      <c r="O7" s="1">
+        <v>6</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V7" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>40459470996</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4432175443</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>17</v>
+      </c>
+      <c r="N8" s="1">
+        <v>20</v>
+      </c>
+      <c r="O8" s="1">
+        <v>6</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V8" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>40459468075</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4432173331</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1">
+        <v>17</v>
+      </c>
+      <c r="N9" s="1">
+        <v>20</v>
+      </c>
+      <c r="O9" s="1">
+        <v>6</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V9" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>40459150647</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4431802813</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>17</v>
+      </c>
+      <c r="N10" s="1">
+        <v>20</v>
+      </c>
+      <c r="O10" s="1">
+        <v>6</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V10" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>40459140053</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4431787925</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>17</v>
+      </c>
+      <c r="N11" s="1">
+        <v>20</v>
+      </c>
+      <c r="O11" s="1">
+        <v>6</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V11" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>40452024469</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4423683284</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>17</v>
+      </c>
+      <c r="N12" s="1">
+        <v>20</v>
+      </c>
+      <c r="O12" s="1">
+        <v>6</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V12" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>40458959058</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4431577360</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <f t="shared" ref="U3" si="2">VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="V3" s="1">
-        <f t="shared" ref="V3" si="3">VLOOKUP(G3,T_TIPO_ENVIO,2,FALSE)</f>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>17</v>
+      </c>
+      <c r="N13" s="1">
+        <v>20</v>
+      </c>
+      <c r="O13" s="1">
+        <v>6</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1">
+        <f t="shared" si="4"/>
         <v>4</v>
+      </c>
+      <c r="V13" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>40454804276</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4426842433</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <v>17</v>
+      </c>
+      <c r="N14" s="1">
+        <v>20</v>
+      </c>
+      <c r="O14" s="1">
+        <v>6</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V14" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>40458383420</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4430925576</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1">
+        <v>17</v>
+      </c>
+      <c r="N15" s="1">
+        <v>20</v>
+      </c>
+      <c r="O15" s="1">
+        <v>6</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V15" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="13" priority="258"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="276"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="12" priority="293"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="311"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="378"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="396"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="10" priority="386"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="404"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="12" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="10" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B2 B4:B1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="577"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="628"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B2 B4:B1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="580"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="631"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 A4:A1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="586"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="634"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 A4:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="589"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="637"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
+  <conditionalFormatting sqref="B3">
     <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1139,7 +2114,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,7 +2169,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1">
         <v>4</v>
@@ -1244,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J27"/>
+  <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:J2"/>
+      <selection activeCell="H2" sqref="H2:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,12 +2231,15 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>40460215902</v>
+      </c>
       <c r="B2">
-        <v>1993</v>
+        <v>4433017396</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1270,86 +2248,418 @@
         <v>34</v>
       </c>
       <c r="F2" s="7">
-        <v>44266</v>
-      </c>
-      <c r="G2" t="s">
+        <v>44271</v>
+      </c>
+      <c r="G2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2">
+        <v>40460215902</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>40460120772</v>
+      </c>
+      <c r="B4">
+        <v>4432906989</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4">
+        <v>40460120772</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40460111549</v>
+      </c>
+      <c r="B5">
+        <v>4432901099</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5">
+        <v>40460111549</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>40459881021</v>
+      </c>
+      <c r="B6">
+        <v>4432634573</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1">
+        <v>40459881021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>40459825586</v>
+      </c>
+      <c r="B7">
+        <v>4432573874</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="1">
+        <v>40459825586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>40459470996</v>
+      </c>
+      <c r="B8">
+        <v>4432175443</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="1">
+        <v>40459470996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>40459468075</v>
+      </c>
+      <c r="B9">
+        <v>4432173331</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="1">
+        <v>40459468075</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>40459150647</v>
+      </c>
+      <c r="B10">
+        <v>4431802813</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="1">
+        <v>40459150647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>40459140053</v>
+      </c>
+      <c r="B11">
+        <v>4431787925</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="1">
+        <v>40459140053</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>40452024469</v>
+      </c>
+      <c r="B12">
+        <v>4423683284</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="1">
+        <v>40452024469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>40458959058</v>
+      </c>
+      <c r="B13">
+        <v>4431577360</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="1">
+        <v>40458959058</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>40454804276</v>
+      </c>
+      <c r="B14">
+        <v>4426842433</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="1">
+        <v>40454804276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>40458383420</v>
+      </c>
+      <c r="B15">
+        <v>4430925576</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="7">
+        <v>44271</v>
+      </c>
+      <c r="G15" t="s">
         <v>35</v>
       </c>
-      <c r="H2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="7">
-        <v>44266</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F5" s="7"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F6" s="7"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F7" s="7"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F8" s="7"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="7"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F10" s="7"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F11" s="7"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="7"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F13" s="7"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F14" s="7"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F15" s="7"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="1">
+        <v>40458383420</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F16" s="7"/>
       <c r="J16" s="1"/>
     </row>
@@ -1391,9 +2701,28 @@
     </row>
     <row r="26" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F26" s="7"/>
+      <c r="J26" s="1"/>
     </row>
     <row r="27" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implementacion de reporte en xlsx para envios desde dash cliente
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNOLOGIA-LOGI\Documents\ALISTAMIENTO\2021\LANCH ALISTAMIENTO MAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNOLOGIA-LOGI\Documents\ALISTAMIENTO\2021\LANCH ALISTAMIENTO ABR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="72">
   <si>
     <t>Guia</t>
   </si>
@@ -228,154 +228,118 @@
     <t>MERCADOLIBRE</t>
   </si>
   <si>
-    <t>MASLOGISTICA - FLEX</t>
-  </si>
-  <si>
-    <t>11D</t>
-  </si>
-  <si>
-    <t>ACCESORIOS CEL VENTA 1993</t>
-  </si>
-  <si>
     <t>CORTESIA</t>
   </si>
   <si>
-    <t>7A</t>
-  </si>
-  <si>
-    <t>EP-TA20JBEUGUS</t>
-  </si>
-  <si>
-    <t>3D</t>
-  </si>
-  <si>
-    <t>EO-IC100BBEGWW</t>
-  </si>
-  <si>
-    <t>FUAP0013</t>
-  </si>
-  <si>
-    <t>7E</t>
-  </si>
-  <si>
-    <t>Jhoan Castellanos</t>
-  </si>
-  <si>
-    <t>Calle 6 C #73-40 / Casa 36 - Las dos avenidas, Kennedy, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>ACS00603</t>
-  </si>
-  <si>
-    <t>3A</t>
-  </si>
-  <si>
-    <t>Yolvan Madrid</t>
-  </si>
-  <si>
-    <t>Cl. 22j #113a-40 / conjunto atahualpa torre 4 apt 307 - Atahualpa, Fontibón, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>ADSG0010</t>
-  </si>
-  <si>
-    <t>8D</t>
-  </si>
-  <si>
-    <t>jose castro</t>
-  </si>
-  <si>
-    <t>Calle 33 A #21B-35S / Casa - Quiroga, Rafael Uribe Uribe, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>076CS27179</t>
-  </si>
-  <si>
-    <t>juliana baez</t>
-  </si>
-  <si>
-    <t>Calle 96 #17-18 / Apartamento 101 - Chico, Chapinero, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>FXXI0021</t>
-  </si>
-  <si>
-    <t>6F</t>
-  </si>
-  <si>
-    <t>danilo ortega sanchez</t>
-  </si>
-  <si>
-    <t>Carrera 70A # 1 - 10-SN / CENTROAMERICAS, Kennedy, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>Yeison Rivera</t>
-  </si>
-  <si>
-    <t>Carrera 94 #42 B 59-SN / Piso 3 - Dindalito, Kennedy, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>ACEC0012</t>
-  </si>
-  <si>
-    <t>3B</t>
-  </si>
-  <si>
-    <t>Manuel Marin</t>
-  </si>
-  <si>
-    <t>Calle 145 #7a-40 / Casa 20 - Belmira, Usaquén, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>milena ruiz</t>
-  </si>
-  <si>
-    <t>calle 185 #49-60 / Casa 80 - mirandela, Suba, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>EP-TA50JBE-BULK</t>
-  </si>
-  <si>
-    <t>11F</t>
-  </si>
-  <si>
-    <t>Lucas Umaña</t>
-  </si>
-  <si>
-    <t>Diagonal 27 #3a-70 / apto 107 - la macarena, Santa Fe, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>FUAP0015</t>
-  </si>
-  <si>
-    <t>1C</t>
-  </si>
-  <si>
-    <t>Sebastian Luna</t>
-  </si>
-  <si>
-    <t>Calle 49h Sur 7a-06 #SN-SN / Es una casa amarilla - Molinos 1, Tunjuelito, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>EF-ZG985CBEGUS</t>
-  </si>
-  <si>
-    <t>Karime David</t>
-  </si>
-  <si>
-    <t>Carrera 9 #52A-20 / Apto. 201 - Marly, Chapinero, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>Tata040 Al</t>
-  </si>
-  <si>
-    <t>Carrera 115 #148-40 / Int 15 501 Flores 1 - Cerca Al Cc Imperial, Suba, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>FXXI0017</t>
-  </si>
-  <si>
-    <t>FUSG0022</t>
+    <t>ACCESORIOS CELULAR</t>
+  </si>
+  <si>
+    <t>042CS20511</t>
+  </si>
+  <si>
+    <t>FLEX</t>
+  </si>
+  <si>
+    <t>042GL20423</t>
+  </si>
+  <si>
+    <t>FSAP0058</t>
+  </si>
+  <si>
+    <t>IGAP0013</t>
+  </si>
+  <si>
+    <t>FUSG0066</t>
+  </si>
+  <si>
+    <t>FUSG0040</t>
+  </si>
+  <si>
+    <t>AGL01511</t>
+  </si>
+  <si>
+    <t>ACS01701</t>
+  </si>
+  <si>
+    <t>IGSG0021</t>
+  </si>
+  <si>
+    <t>FXXI0029</t>
+  </si>
+  <si>
+    <t>ESXI0005</t>
+  </si>
+  <si>
+    <t>000GL21813</t>
+  </si>
+  <si>
+    <t>XDAP0017</t>
+  </si>
+  <si>
+    <t>Virgilio Diaz</t>
+  </si>
+  <si>
+    <t>Calle 123 #47-09 / Apartamento 204 (Edificio Nekko) - Batan, Suba, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>marina bernal</t>
+  </si>
+  <si>
+    <t>Carrera 54 #57B-37 / Bloque C3 Apto.405 - Pablo sexto Etapa 1, Teusaquillo, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Yolinda Cristancho</t>
+  </si>
+  <si>
+    <t>carrera99bis #14a-61 / urbanizacion pueblo nuevo dos casa 125 - fontibon zona franca, Fontibón, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Paola Pedreros</t>
+  </si>
+  <si>
+    <t>Carrera 89 #22B-96 / Bloque R Interior 3 Apto 406 - Fontibon, Fontibón, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Valentina Tobon</t>
+  </si>
+  <si>
+    <t>Calle 101 #20-24 / Casa 1 - Chicó, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Julian Gutierrez Florez</t>
+  </si>
+  <si>
+    <t>Calle 114A #15A-70 / Apto. 203 Edif. Atardezzer - Santa Barbara Central, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>JONATHAN MINA MOSQUERA</t>
+  </si>
+  <si>
+    <t>Cra 79a #11b-40 / Torre G Apto 203 Conjunto Caminos Del Parque 2 - Castilla, Kennedy, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>hernandez arias daniel fernando</t>
+  </si>
+  <si>
+    <t>Calle 159 #7-74 / Torre 2 apartamento 1511 - Barrancas norte, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Gabriel Narvaez</t>
+  </si>
+  <si>
+    <t>Calle 165B #14A-07 / Torre 2, Apartamento 1313, Parques De San Martin - Pradera Norte, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Dag Nagoda</t>
+  </si>
+  <si>
+    <t>Calle Calle 96 #9-69-SN / Apto 801 - Chapinero, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>carlos francisco rubio sanchez</t>
+  </si>
+  <si>
+    <t>Cra 19 A #122-85 / Apto 606, Edificio San José - Santa Barbara, Usaquén, Bogotá D.C.</t>
   </si>
 </sst>
 </file>
@@ -509,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -526,6 +490,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,6 +501,46 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -591,46 +598,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1004,7 +971,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1103,13 +1070,13 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>40460215902</v>
+        <v>40506110880</v>
       </c>
       <c r="B2" s="1">
-        <v>4433017396</v>
+        <v>4485275771</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1124,10 +1091,10 @@
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -1154,7 +1121,7 @@
         <v>29</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -1170,13 +1137,13 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>40460215902</v>
+        <v>40506110880</v>
       </c>
       <c r="B3" s="1">
-        <v>4433017396</v>
+        <v>4485275771</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -1190,12 +1157,8 @@
       <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="1">
         <v>0</v>
       </c>
@@ -1221,7 +1184,7 @@
         <v>29</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S3" s="1">
         <v>0</v>
@@ -1237,13 +1200,13 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>40460120772</v>
+        <v>40505835775</v>
       </c>
       <c r="B4" s="1">
-        <v>4432906989</v>
+        <v>4484965180</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1258,10 +1221,10 @@
         <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -1288,7 +1251,7 @@
         <v>29</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S4" s="1">
         <v>0</v>
@@ -1305,13 +1268,13 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>40460111549</v>
+        <v>40505835775</v>
       </c>
       <c r="B5" s="1">
-        <v>4432901099</v>
+        <v>4484965180</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1325,12 +1288,8 @@
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1">
         <v>0</v>
       </c>
@@ -1356,30 +1315,30 @@
         <v>29</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1">
-        <f t="shared" ref="U5:U15" si="4">VLOOKUP(E5,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" ref="U5:U16" si="4">VLOOKUP(E5,T_OPERADORES,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="V5" s="1">
-        <f t="shared" ref="V5:V15" si="5">VLOOKUP(G5,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="V5:V16" si="5">VLOOKUP(G5,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>40459881021</v>
+        <v>40504598948</v>
       </c>
       <c r="B6" s="1">
-        <v>4432634573</v>
+        <v>4483558475</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1394,10 +1353,10 @@
         <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
@@ -1424,7 +1383,7 @@
         <v>29</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S6" s="1">
         <v>0</v>
@@ -1441,13 +1400,13 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>40459825586</v>
+        <v>40505562859</v>
       </c>
       <c r="B7" s="1">
-        <v>4432573874</v>
+        <v>4484647731</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -1462,10 +1421,10 @@
         <v>24</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
@@ -1492,7 +1451,7 @@
         <v>29</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S7" s="1">
         <v>0</v>
@@ -1509,13 +1468,13 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>40459470996</v>
+        <v>40505418672</v>
       </c>
       <c r="B8" s="1">
-        <v>4432175443</v>
+        <v>4484488620</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1530,10 +1489,10 @@
         <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
@@ -1560,7 +1519,7 @@
         <v>29</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S8" s="1">
         <v>0</v>
@@ -1577,13 +1536,13 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>40459468075</v>
+        <v>40505418672</v>
       </c>
       <c r="B9" s="1">
-        <v>4432173331</v>
+        <v>4484488620</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1597,12 +1556,8 @@
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1">
         <v>0</v>
       </c>
@@ -1628,7 +1583,7 @@
         <v>29</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
@@ -1645,13 +1600,13 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>40459150647</v>
+        <v>40505113400</v>
       </c>
       <c r="B10" s="1">
-        <v>4431802813</v>
+        <v>4484137933</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1666,10 +1621,10 @@
         <v>24</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J10" s="1">
         <v>0</v>
@@ -1696,7 +1651,7 @@
         <v>29</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
@@ -1713,13 +1668,13 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>40459140053</v>
+        <v>40505113400</v>
       </c>
       <c r="B11" s="1">
-        <v>4431787925</v>
+        <v>4484137933</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1733,12 +1688,8 @@
       <c r="G11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1">
         <v>0</v>
       </c>
@@ -1764,7 +1715,7 @@
         <v>29</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S11" s="1">
         <v>0</v>
@@ -1781,13 +1732,13 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>40452024469</v>
+        <v>40505091463</v>
       </c>
       <c r="B12" s="1">
-        <v>4423683284</v>
+        <v>4484117675</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -1802,10 +1753,10 @@
         <v>24</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
@@ -1832,7 +1783,7 @@
         <v>29</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S12" s="1">
         <v>0</v>
@@ -1849,13 +1800,13 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>40458959058</v>
+        <v>40504903688</v>
       </c>
       <c r="B13" s="1">
-        <v>4431577360</v>
+        <v>4483901430</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1870,10 +1821,10 @@
         <v>24</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
@@ -1900,7 +1851,7 @@
         <v>29</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S13" s="1">
         <v>0</v>
@@ -1917,13 +1868,13 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>40454804276</v>
+        <v>40504785631</v>
       </c>
       <c r="B14" s="1">
-        <v>4426842433</v>
+        <v>4483771102</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1938,10 +1889,10 @@
         <v>24</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
@@ -1968,7 +1919,7 @@
         <v>29</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S14" s="1">
         <v>0</v>
@@ -1985,13 +1936,13 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>40458383420</v>
+        <v>40504585148</v>
       </c>
       <c r="B15" s="1">
-        <v>4430925576</v>
+        <v>4483537926</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -2006,10 +1957,10 @@
         <v>24</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="J15" s="1">
         <v>0</v>
@@ -2036,7 +1987,7 @@
         <v>29</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S15" s="1">
         <v>0</v>
@@ -2051,57 +2002,125 @@
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>40504460547</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4483403557</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>17</v>
+      </c>
+      <c r="N16" s="1">
+        <v>20</v>
+      </c>
+      <c r="O16" s="1">
+        <v>6</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V16" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="16" priority="276"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="330"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="15" priority="311"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="365"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="396"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="450"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="13" priority="404"/>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="13" priority="458"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="12" priority="22"/>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="12" priority="76"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="11" priority="77"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="10" priority="24"/>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="10" priority="78"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B2 B4:B1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="628"/>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="9" priority="58"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B2 B4:B1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="631"/>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="8" priority="55"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="7" priority="56"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="6" priority="57"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="5" priority="59"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="4" priority="60"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="774"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="777"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 A4:A1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="634"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="798"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 A4:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="637"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="801"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2124,14 +2143,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="9"/>
+      <c r="D1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="8"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2169,7 +2188,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1">
         <v>4</v>
@@ -2219,10 +2238,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J33"/>
+  <dimension ref="A2:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I15"/>
+      <selection activeCell="K2" sqref="K2:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,498 +2250,449 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40460215902</v>
+        <v>40506110880</v>
       </c>
       <c r="B2">
-        <v>4433017396</v>
+        <v>4485275771</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F2" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H2" t="s">
+        <v>44295</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2">
+        <v>40506110880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>40505835775</v>
+      </c>
+      <c r="B4">
+        <v>4484965180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4">
+        <v>40505835775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>40504598948</v>
+      </c>
+      <c r="B6">
+        <v>4483558475</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6">
+        <v>40504598948</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>40505562859</v>
+      </c>
+      <c r="B7">
+        <v>4484647731</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7">
+        <v>40505562859</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>40505418672</v>
+      </c>
+      <c r="B8">
+        <v>4484488620</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8">
+        <v>40505418672</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>40505113400</v>
+      </c>
+      <c r="B10">
+        <v>4484137933</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10">
+        <v>40505113400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="I2" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>40505091463</v>
+      </c>
+      <c r="B12">
+        <v>4484117675</v>
+      </c>
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="J2">
-        <v>40460215902</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>40460120772</v>
-      </c>
-      <c r="B4">
-        <v>4432906989</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12">
+        <v>40505091463</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>40504903688</v>
+      </c>
+      <c r="B13">
+        <v>4483901430</v>
+      </c>
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13">
+        <v>40504903688</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>40504785631</v>
+      </c>
+      <c r="B14">
+        <v>4483771102</v>
+      </c>
+      <c r="C14" t="s">
         <v>47</v>
       </c>
-      <c r="H4" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14">
+        <v>40504785631</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>40504585148</v>
+      </c>
+      <c r="B15">
+        <v>4483537926</v>
+      </c>
+      <c r="C15" t="s">
         <v>48</v>
       </c>
-      <c r="I4" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="7">
+        <v>44295</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15">
+        <v>40504585148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>40504460547</v>
+      </c>
+      <c r="B16">
+        <v>4483403557</v>
+      </c>
+      <c r="C16" t="s">
         <v>49</v>
       </c>
-      <c r="J4">
-        <v>40460120772</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>40460111549</v>
-      </c>
-      <c r="B5">
-        <v>4432901099</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5">
-        <v>40460111549</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>40459881021</v>
-      </c>
-      <c r="B6">
-        <v>4432634573</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="1">
-        <v>40459881021</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>40459825586</v>
-      </c>
-      <c r="B7">
-        <v>4432573874</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="1">
-        <v>40459825586</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>40459470996</v>
-      </c>
-      <c r="B8">
-        <v>4432175443</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="1">
-        <v>40459470996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>40459468075</v>
-      </c>
-      <c r="B9">
-        <v>4432173331</v>
-      </c>
-      <c r="C9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="1">
-        <v>40459468075</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>40459150647</v>
-      </c>
-      <c r="B10">
-        <v>4431802813</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" s="1">
-        <v>40459150647</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>40459140053</v>
-      </c>
-      <c r="B11">
-        <v>4431787925</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="7">
+        <v>44295</v>
+      </c>
+      <c r="K16" t="s">
         <v>70</v>
       </c>
-      <c r="H11" t="s">
+      <c r="L16" t="s">
         <v>71</v>
       </c>
-      <c r="I11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" s="1">
-        <v>40459140053</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>40452024469</v>
-      </c>
-      <c r="B12">
-        <v>4423683284</v>
-      </c>
-      <c r="C12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="1">
-        <v>40452024469</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>40458959058</v>
-      </c>
-      <c r="B13">
-        <v>4431577360</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="1">
-        <v>40458959058</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>40454804276</v>
-      </c>
-      <c r="B14">
-        <v>4426842433</v>
-      </c>
-      <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G14" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J14" s="1">
-        <v>40454804276</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>40458383420</v>
-      </c>
-      <c r="B15">
-        <v>4430925576</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="7">
-        <v>44271</v>
-      </c>
-      <c r="G15" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" t="s">
-        <v>81</v>
-      </c>
-      <c r="J15" s="1">
-        <v>40458383420</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F16" s="7"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>40504460547</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F17" s="7"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18" s="7"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19" s="7"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F20" s="7"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F21" s="7"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F22" s="7"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F23" s="7"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F24" s="7"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F25" s="7"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="6:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F26" s="7"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
optimizacion de control al gestionar ventas en alistamiento
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="77">
   <si>
     <t>Guia</t>
   </si>
@@ -240,106 +240,121 @@
     <t>FLEX</t>
   </si>
   <si>
+    <t>OXAP0017</t>
+  </si>
+  <si>
+    <t>ASD00841</t>
+  </si>
+  <si>
+    <t>EP-TA800XBEGUS</t>
+  </si>
+  <si>
+    <t>ASD00840</t>
+  </si>
+  <si>
+    <t>ASD00839</t>
+  </si>
+  <si>
+    <t>FXXI0017</t>
+  </si>
+  <si>
+    <t>orlando silva</t>
+  </si>
+  <si>
+    <t>Av Calle 80 #102 64-SN / torre 36 apto 205 - Bochica, Engativá, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Jorge Pulido</t>
+  </si>
+  <si>
+    <t>Carrera 16 #143-94 / Apartamento 501 - Cedritos, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>EP-TA20JBEUGUS</t>
+  </si>
+  <si>
+    <t>Jinneth Murillo</t>
+  </si>
+  <si>
+    <t>Calle 71B Sur #78A-16 / Casa C - Jose Maria Carbonel, Bosa, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>AGL01511</t>
+  </si>
+  <si>
+    <t>Waldir Martinez</t>
+  </si>
+  <si>
+    <t>Calle 46 #03-35 / Apto 214 - Chapinero Alto, Chapinero, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>gabriel beltran</t>
+  </si>
+  <si>
+    <t>Calle 45a sur #47a-42 / Cadete Diego Andres Rojas Rios, compañia santander,cc: 1005230212 - rafael uribe uribe, ECSAN, Tunjuelito, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>DWSG0010</t>
+  </si>
+  <si>
+    <t>Fabian Hernandez</t>
+  </si>
+  <si>
+    <t>Calle 64c #120-65 / La esperanza, Engativá, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>XDSG0024</t>
+  </si>
+  <si>
+    <t>GUSTAVO ADOLFO CORREA DUQUE</t>
+  </si>
+  <si>
+    <t>Cra 12 Este #11 Sur-25 / Torre 7 Apto 302 - San Cristobal Sur, San Cristobal Sur, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Paula Andrea Castaño Forero</t>
+  </si>
+  <si>
+    <t>calle 130c #59 d-75 / Torre 1 apto 307 - Suba, Sotileza, Suba, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Cesar Sua</t>
+  </si>
+  <si>
+    <t>Calle 61 #3a-46 / Apto 206 - La salle, Chapinero, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FXOP0015</t>
+  </si>
+  <si>
+    <t>CARLOS ANDRES SEDANO</t>
+  </si>
+  <si>
+    <t>Diagonal 91 #87-59 / Casa 5 - La Serena, Engativá, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Juan c RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>Calle 107 A #13-29 / Apartamento 205 - SanTa Paula, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Virgilio Diaz</t>
+  </si>
+  <si>
+    <t>Calle 123 #47-09</t>
+  </si>
+  <si>
     <t>042GL20423</t>
   </si>
   <si>
-    <t>FSAP0058</t>
-  </si>
-  <si>
-    <t>IGAP0013</t>
-  </si>
-  <si>
-    <t>FUSG0066</t>
-  </si>
-  <si>
-    <t>FUSG0040</t>
-  </si>
-  <si>
-    <t>AGL01511</t>
-  </si>
-  <si>
-    <t>ACS01701</t>
-  </si>
-  <si>
-    <t>IGSG0021</t>
-  </si>
-  <si>
-    <t>FXXI0029</t>
-  </si>
-  <si>
-    <t>ESXI0005</t>
-  </si>
-  <si>
-    <t>000GL21813</t>
-  </si>
-  <si>
-    <t>XDAP0017</t>
-  </si>
-  <si>
-    <t>Virgilio Diaz</t>
-  </si>
-  <si>
-    <t>Calle 123 #47-09 / Apartamento 204 (Edificio Nekko) - Batan, Suba, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>marina bernal</t>
-  </si>
-  <si>
-    <t>Carrera 54 #57B-37 / Bloque C3 Apto.405 - Pablo sexto Etapa 1, Teusaquillo, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>Yolinda Cristancho</t>
-  </si>
-  <si>
-    <t>carrera99bis #14a-61 / urbanizacion pueblo nuevo dos casa 125 - fontibon zona franca, Fontibón, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>Paola Pedreros</t>
-  </si>
-  <si>
-    <t>Carrera 89 #22B-96 / Bloque R Interior 3 Apto 406 - Fontibon, Fontibón, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>Valentina Tobon</t>
-  </si>
-  <si>
-    <t>Calle 101 #20-24 / Casa 1 - Chicó, Usaquén, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>Julian Gutierrez Florez</t>
-  </si>
-  <si>
-    <t>Calle 114A #15A-70 / Apto. 203 Edif. Atardezzer - Santa Barbara Central, Usaquén, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>JONATHAN MINA MOSQUERA</t>
-  </si>
-  <si>
-    <t>Cra 79a #11b-40 / Torre G Apto 203 Conjunto Caminos Del Parque 2 - Castilla, Kennedy, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>hernandez arias daniel fernando</t>
-  </si>
-  <si>
-    <t>Calle 159 #7-74 / Torre 2 apartamento 1511 - Barrancas norte, Usaquén, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>Gabriel Narvaez</t>
-  </si>
-  <si>
-    <t>Calle 165B #14A-07 / Torre 2, Apartamento 1313, Parques De San Martin - Pradera Norte, Usaquén, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>Dag Nagoda</t>
-  </si>
-  <si>
-    <t>Calle Calle 96 #9-69-SN / Apto 801 - Chapinero, Bogotá D.C.</t>
-  </si>
-  <si>
-    <t>carlos francisco rubio sanchez</t>
-  </si>
-  <si>
-    <t>Cra 19 A #122-85 / Apto 606, Edificio San José - Santa Barbara, Usaquén, Bogotá D.C.</t>
+    <t>043CS20525</t>
+  </si>
+  <si>
+    <t>NEPTALI E BARRIOS V</t>
+  </si>
+  <si>
+    <t>Calle 67 #4-40 / Apto 205, Edificio Evropa - Nueva Granada, Chapinero, Bogotá D.C.</t>
   </si>
 </sst>
 </file>
@@ -975,7 +990,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,13 +1085,13 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>40506110880</v>
+        <v>40513807365</v>
       </c>
       <c r="B2" s="1">
-        <v>4485275771</v>
+        <v>4494033400</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1091,10 +1106,10 @@
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -1137,13 +1152,13 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>40506110880</v>
+        <v>40513764999</v>
       </c>
       <c r="B3" s="1">
-        <v>4485275771</v>
+        <v>4493986240</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -1157,8 +1172,12 @@
       <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="J3" s="1">
         <v>0</v>
       </c>
@@ -1200,13 +1219,13 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>40505835775</v>
+        <v>40513403099</v>
       </c>
       <c r="B4" s="1">
-        <v>4484965180</v>
+        <v>4493577573</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1221,10 +1240,10 @@
         <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -1268,13 +1287,13 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>40505835775</v>
+        <v>40512640377</v>
       </c>
       <c r="B5" s="1">
-        <v>4484965180</v>
+        <v>4492691942</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1288,8 +1307,12 @@
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="J5" s="1">
         <v>0</v>
       </c>
@@ -1332,13 +1355,13 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>40504598948</v>
+        <v>40512360815</v>
       </c>
       <c r="B6" s="1">
-        <v>4483558475</v>
+        <v>4492372795</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1400,13 +1423,13 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>40505562859</v>
+        <v>40512252090</v>
       </c>
       <c r="B7" s="1">
-        <v>4484647731</v>
+        <v>4492259587</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -1421,10 +1444,10 @@
         <v>24</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
@@ -1468,13 +1491,13 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>40505418672</v>
+        <v>40512028599</v>
       </c>
       <c r="B8" s="1">
-        <v>4484488620</v>
+        <v>4492004978</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1489,10 +1512,10 @@
         <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
@@ -1536,13 +1559,13 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>40505418672</v>
+        <v>40511952620</v>
       </c>
       <c r="B9" s="1">
-        <v>4484488620</v>
+        <v>4491920532</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1556,8 +1579,12 @@
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="J9" s="1">
         <v>0</v>
       </c>
@@ -1600,13 +1627,13 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>40505113400</v>
+        <v>40511952620</v>
       </c>
       <c r="B10" s="1">
-        <v>4484137933</v>
+        <v>4491920532</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1621,10 +1648,10 @@
         <v>24</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J10" s="1">
         <v>0</v>
@@ -1668,13 +1695,13 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>40505113400</v>
+        <v>40511938561</v>
       </c>
       <c r="B11" s="1">
-        <v>4484137933</v>
+        <v>4491908351</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1688,8 +1715,12 @@
       <c r="G11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="J11" s="1">
         <v>0</v>
       </c>
@@ -1732,13 +1763,13 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>40505091463</v>
+        <v>40511836169</v>
       </c>
       <c r="B12" s="1">
-        <v>4484117675</v>
+        <v>4491790543</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -1753,10 +1784,10 @@
         <v>24</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
@@ -1800,13 +1831,13 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>40504903688</v>
+        <v>40511821285</v>
       </c>
       <c r="B13" s="1">
-        <v>4483901430</v>
+        <v>4491775111</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1821,10 +1852,10 @@
         <v>24</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
@@ -1868,13 +1899,13 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>40504785631</v>
+        <v>40511588275</v>
       </c>
       <c r="B14" s="1">
-        <v>4483771102</v>
+        <v>4491510524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1889,10 +1920,10 @@
         <v>24</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
@@ -1936,13 +1967,13 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>40504585148</v>
+        <v>40511588275</v>
       </c>
       <c r="B15" s="1">
-        <v>4483537926</v>
+        <v>4491510524</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1957,10 +1988,10 @@
         <v>24</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J15" s="1">
         <v>0</v>
@@ -2004,13 +2035,13 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>40504460547</v>
+        <v>40511729292</v>
       </c>
       <c r="B16" s="1">
-        <v>4483403557</v>
+        <v>4491665980</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -2025,10 +2056,10 @@
         <v>24</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="J16" s="1">
         <v>0</v>
@@ -2072,55 +2103,55 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="16" priority="330"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="332"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="15" priority="365"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="367"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="450"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="452"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="13" priority="458"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="460"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="12" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="11" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="10" priority="78"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="9" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="8" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="7" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="6" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="5" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="4" priority="60"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="774"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="776"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="777"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="779"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 A4:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="798"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="800"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 A4:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="801"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="803"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2238,7 +2269,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M34"/>
+  <dimension ref="A2:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2:L16"/>
@@ -2250,15 +2281,15 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40506110880</v>
+        <v>40513807365</v>
       </c>
       <c r="B2">
-        <v>4485275771</v>
+        <v>4494033400</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2267,22 +2298,25 @@
         <v>37</v>
       </c>
       <c r="F2" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2">
-        <v>40506110880</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>40513764999</v>
+      </c>
+      <c r="B3">
+        <v>4493986240</v>
+      </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2291,19 +2325,25 @@
         <v>37</v>
       </c>
       <c r="F3" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40505835775</v>
+        <v>40513403099</v>
       </c>
       <c r="B4">
-        <v>4484965180</v>
+        <v>4493577573</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2312,22 +2352,25 @@
         <v>37</v>
       </c>
       <c r="F4" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4">
-        <v>40505835775</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40512640377</v>
+      </c>
+      <c r="B5">
+        <v>4492691942</v>
+      </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2336,19 +2379,25 @@
         <v>37</v>
       </c>
       <c r="F5" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40504598948</v>
+        <v>40512360815</v>
       </c>
       <c r="B6">
-        <v>4483558475</v>
+        <v>4492372795</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2357,7 +2406,7 @@
         <v>37</v>
       </c>
       <c r="F6" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" t="s">
@@ -2366,19 +2415,16 @@
       <c r="L6" t="s">
         <v>55</v>
       </c>
-      <c r="M6">
-        <v>40504598948</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40505562859</v>
+        <v>40512252090</v>
       </c>
       <c r="B7">
-        <v>4484647731</v>
+        <v>4492259587</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2387,28 +2433,25 @@
         <v>37</v>
       </c>
       <c r="F7" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7">
-        <v>40505562859</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40505418672</v>
+        <v>40512028599</v>
       </c>
       <c r="B8">
-        <v>4484488620</v>
+        <v>4492004978</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2417,22 +2460,25 @@
         <v>37</v>
       </c>
       <c r="F8" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L8" t="s">
-        <v>59</v>
-      </c>
-      <c r="M8">
-        <v>40505418672</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>40511952620</v>
+      </c>
+      <c r="B9">
+        <v>4491920532</v>
+      </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2441,19 +2487,19 @@
         <v>37</v>
       </c>
       <c r="F9" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>40505113400</v>
-      </c>
-      <c r="B10">
-        <v>4484137933</v>
-      </c>
+      <c r="K9" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2462,22 +2508,19 @@
         <v>37</v>
       </c>
       <c r="F10" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" t="s">
-        <v>60</v>
-      </c>
-      <c r="L10" t="s">
-        <v>61</v>
-      </c>
-      <c r="M10">
-        <v>40505113400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>40511938561</v>
+      </c>
+      <c r="B11">
+        <v>4491908351</v>
+      </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2486,19 +2529,25 @@
         <v>37</v>
       </c>
       <c r="F11" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40505091463</v>
+        <v>40511836169</v>
       </c>
       <c r="B12">
-        <v>4484117675</v>
+        <v>4491790543</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2507,28 +2556,25 @@
         <v>37</v>
       </c>
       <c r="F12" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="L12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M12">
-        <v>40505091463</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40504903688</v>
+        <v>40511821285</v>
       </c>
       <c r="B13">
-        <v>4483901430</v>
+        <v>4491775111</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2537,28 +2583,25 @@
         <v>37</v>
       </c>
       <c r="F13" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L13" t="s">
-        <v>65</v>
-      </c>
-      <c r="M13">
-        <v>40504903688</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>40504785631</v>
+        <v>40511588275</v>
       </c>
       <c r="B14">
-        <v>4483771102</v>
+        <v>4491510524</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2567,28 +2610,19 @@
         <v>37</v>
       </c>
       <c r="F14" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
-      </c>
-      <c r="M14">
-        <v>40504785631</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>40504585148</v>
-      </c>
-      <c r="B15">
-        <v>4483537926</v>
-      </c>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2597,28 +2631,19 @@
         <v>37</v>
       </c>
       <c r="F15" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" t="s">
-        <v>68</v>
-      </c>
-      <c r="L15" t="s">
-        <v>69</v>
-      </c>
-      <c r="M15">
-        <v>40504585148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>40504460547</v>
+        <v>40511729292</v>
       </c>
       <c r="B16">
-        <v>4483403557</v>
+        <v>4491665980</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2627,16 +2652,13 @@
         <v>37</v>
       </c>
       <c r="F16" s="7">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="K16" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="L16" t="s">
-        <v>71</v>
-      </c>
-      <c r="M16">
-        <v>40504460547</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
actualizacion de vistas dash board servicios cambio en controlador al guardar estados de aenvio
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3.xlsx
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="T_OPERADORES">Hoja2!$A$1:$B$8</definedName>
-    <definedName name="T_TIPO_ENVIO">Hoja2!$D$1:$E$3</definedName>
+    <definedName name="T_TIPO_ENVIO">Hoja2!$D$1:$E$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="148">
   <si>
     <t>Guia</t>
   </si>
@@ -180,6 +180,9 @@
     <t>OPERADORES</t>
   </si>
   <si>
+    <t>INTERAPIDISIMO</t>
+  </si>
+  <si>
     <t>TIPO ENVIO</t>
   </si>
   <si>
@@ -243,21 +246,252 @@
     <t>MERCADOLIBRE</t>
   </si>
   <si>
+    <t>CORTESIA</t>
+  </si>
+  <si>
     <t>ACCESORIOS CELULAR</t>
   </si>
   <si>
-    <t>INTERRAPIDISIMO</t>
-  </si>
-  <si>
-    <t>XDXI0017</t>
-  </si>
-  <si>
-    <t>FXHW0020</t>
+    <t>FLEX</t>
+  </si>
+  <si>
+    <t>EP-DG950CBE-BULK</t>
+  </si>
+  <si>
+    <t>ACEC0013</t>
+  </si>
+  <si>
+    <t>FXXI0029</t>
+  </si>
+  <si>
+    <t>042CS20511</t>
+  </si>
+  <si>
+    <t>camilo gomez</t>
+  </si>
+  <si>
+    <t>Carrera 81 D #8C-51 / Apartamento 401 - Valladolid - Castilla, Fontibón, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>EP-TA800XBEGUS</t>
+  </si>
+  <si>
+    <t>juan andrade</t>
+  </si>
+  <si>
+    <t>Carrera 4 #24-59 / Conjunto Torres Blancas - Centro, Santa Fe, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>hernandez arias daniel fernando</t>
+  </si>
+  <si>
+    <t>Calle 159 #7-74 / Torre 2 apartamento 1511 - Barrancas norte, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>XDXI0008</t>
+  </si>
+  <si>
+    <t>ANDRES FELIPE DUSSAN TOVAR</t>
+  </si>
+  <si>
+    <t>CALLE 12C #71C-30 / conjunto residencial torres de villa alsacia, torre 10 - apartamento 504 - ALSACIA, Kennedy, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>ESXI0005</t>
+  </si>
+  <si>
+    <t>FSSG0090</t>
+  </si>
+  <si>
+    <t>jennifer Maria Piñerez</t>
+  </si>
+  <si>
+    <t>Cr 4 # 16-15 #SN-SN / Torre Bicentenario Apt 1005 - Centro, La Candelaria, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>XMAP0004</t>
+  </si>
+  <si>
+    <t>Lucía Martínez</t>
+  </si>
+  <si>
+    <t>Calle 96 #46-58 / APTO 633 INT 3 - LA CASTELLANA, Barrios Unidos, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Jose Leonardo Guerrero Cardozo</t>
+  </si>
+  <si>
+    <t>Carrera 9 #140-93 / APARTAMENTO 401 - Cedritos, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>ASD00540</t>
+  </si>
+  <si>
+    <t>Hawyn Diaz</t>
+  </si>
+  <si>
+    <t>Calle 71a #20-78 / Apartamento 302 - Colombia, Barrios Unidos, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FUAP0005</t>
+  </si>
+  <si>
+    <t>ESAP0004</t>
+  </si>
+  <si>
+    <t>XDSG0044</t>
+  </si>
+  <si>
+    <t>Álvaro José Bocanegra Pérez</t>
+  </si>
+  <si>
+    <t>Carrera 7a #151-37 / Interior 1 - Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>SLSG0043</t>
+  </si>
+  <si>
+    <t>John Garzon Contreras</t>
+  </si>
+  <si>
+    <t>Calle 17 sur #39-95 / Int 3 apto 402 - El remanso, Puente Aranda, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FUSG0021</t>
+  </si>
+  <si>
+    <t>CARLOS IBARGUEN</t>
+  </si>
+  <si>
+    <t>Carrera 79 #19A-86 / APTO 301 TORRE 1 C.R. El Remanso - LA FELICIDAD, Fontibón, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Ivan Romero</t>
+  </si>
+  <si>
+    <t>Trans 4 Este #61-05 / Torre 3 Apt 1507 Conjunto Sierras del Este - Chapinero, Chapinero, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FXXI0028</t>
+  </si>
+  <si>
+    <t>Karen Bastidas</t>
+  </si>
+  <si>
+    <t>Carrera 69 #47-50 / Edificio Entre Verde Torre 1 Apto 703 - Jardín Botánico, Engativá, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>David Leonardo Rodríguez Montaño</t>
+  </si>
+  <si>
+    <t>Calle 52g #37a-22 / Casa dos pisos - Fatima, Tunjuelito, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FXXI0003</t>
+  </si>
+  <si>
+    <t>camilo murillo sanchez</t>
+  </si>
+  <si>
+    <t>Calle 38 sur #72P-68 / Brr. Carvajal Carimagua/ Preguntar x German Romero - Carvajal, Kennedy, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>RWSP040</t>
+  </si>
+  <si>
+    <t>Andres Ospina</t>
+  </si>
+  <si>
+    <t>Cll 26 sur #68F-26 / Casa - La LLanura, Teusaquillo, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>064GL24527</t>
+  </si>
+  <si>
+    <t>Maryori Fajardo G</t>
+  </si>
+  <si>
+    <t>Av Calle 26 #27-16 / Edificio Portal del Parque APTO 401 - Teusaquillo, Teusaquillo, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FSSG0084</t>
+  </si>
+  <si>
+    <t>Damiano Nocera</t>
+  </si>
+  <si>
+    <t>Carrera 16 #106-45 / En Porteria - San Patricio, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Benjamin Pabon Rodríguez</t>
+  </si>
+  <si>
+    <t>Barrio Catalina II Calle 52A Sur Nro. 77P-66 #SN-SN / 3 er Piso - Kennedy, Bogotá D.C.</t>
   </si>
   <si>
     <t>EP-TA50JBE-BULK</t>
   </si>
   <si>
+    <t>Camilo Alarcón</t>
+  </si>
+  <si>
+    <t>cl 104b #54-07 / apto 202 - Puentelargo, Suba, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Cristian Fernando Tovar</t>
+  </si>
+  <si>
+    <t>Calle 12A #71C-20 / Torre 7 Apto 1004 Oviedo - Villa Alsacia, Kennedy, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FUAP0015</t>
+  </si>
+  <si>
+    <t>Jose Gabriel Rodriguez Narvaez</t>
+  </si>
+  <si>
+    <t>Carrera 14 #77a-61 / Conjunto Paseo del Lago torre norte apto 603 - El Lago, Chapinero, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>FUSG0040</t>
+  </si>
+  <si>
+    <t>Wilmer Sanguino</t>
+  </si>
+  <si>
+    <t>Carrera 9 # 124-30 Local 2</t>
+  </si>
+  <si>
+    <t>320 2562775</t>
+  </si>
+  <si>
+    <t>DWSG0002</t>
+  </si>
+  <si>
+    <t>062CS24469</t>
+  </si>
+  <si>
+    <t>sebastian cabarcas</t>
+  </si>
+  <si>
+    <t>Calle80 # 38-00 escuela militar de cadetes porfavor llamar antes de entrgar ya que es una unidad militar</t>
+  </si>
+  <si>
+    <t>310 5542791</t>
+  </si>
+  <si>
+    <t>Henry Barrero</t>
+  </si>
+  <si>
+    <t>Cr 22 #120-52</t>
+  </si>
+  <si>
+    <t>GONZALO MENDIOLA</t>
+  </si>
+  <si>
+    <t>CALLE 169 A #56-35</t>
+  </si>
+  <si>
     <t>Recaudo</t>
   </si>
   <si>
@@ -265,6 +499,93 @@
   </si>
   <si>
     <t>Valor Pago</t>
+  </si>
+  <si>
+    <t>OXSG0027</t>
+  </si>
+  <si>
+    <t>XDSG0026</t>
+  </si>
+  <si>
+    <t>ASD00542</t>
+  </si>
+  <si>
+    <t>XDSG0046</t>
+  </si>
+  <si>
+    <t>FSSG0078</t>
+  </si>
+  <si>
+    <t>XDOP0007</t>
+  </si>
+  <si>
+    <t>043CS20525</t>
+  </si>
+  <si>
+    <t>EF-ZN980CBEGUS</t>
+  </si>
+  <si>
+    <t>ESAP0003</t>
+  </si>
+  <si>
+    <t>Giovanni Vellojin</t>
+  </si>
+  <si>
+    <t>Calle 128 B #19-16 / Edificio Saint Thomas APT 1107 - la calleja, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Johnattan Daza</t>
+  </si>
+  <si>
+    <t>calle 169b #75-60 / Altos de la Colina Torre 5 apto 1401 - Pradera Norte, Usaquén, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>LUZ ADRIANA GARZON ZABALA</t>
+  </si>
+  <si>
+    <t>Transversal 76D #81B-36 / Casa - Minuto de Dios, Engativá, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Erney Giovanny Villamil</t>
+  </si>
+  <si>
+    <t>Carrera 86 #76-32 / Asadero - La Granja, Engativá, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Cristian David Arias Correa</t>
+  </si>
+  <si>
+    <t>Calle 55 Sur #24C-28 / Condados de Santa Lucía III - Torre 1 - Apartamento 501 - Tunjuelito, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Jhoan Sebastián Salazar Montoya</t>
+  </si>
+  <si>
+    <t>Calle 23D #82-71 / Interior 3 - 512 - Fontibón, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Brayan David Vela</t>
+  </si>
+  <si>
+    <t>Carrera 52 #14-40 / Conjunto La Fontana Torre 1 Apto 105 - Puente Aranda, Puente Aranda, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Dennis Fabian Bejarano</t>
+  </si>
+  <si>
+    <t>Calle 32 #6a-15 / Apartamento 1708 Ed. Equilibrium - San Martin, Santa Fe, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>JUAN SEBASTIAN RIVERA</t>
+  </si>
+  <si>
+    <t>CALLE 90 #94p-45 / int. 108 - bachue, Engativá, Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>Bertha Vargas</t>
+  </si>
+  <si>
+    <t>Calle 57z sur #75d 07casa 146 - Ciudad Bolivar</t>
   </si>
 </sst>
 </file>
@@ -404,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -421,7 +742,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -429,11 +752,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -441,6 +766,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -466,11 +801,41 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -496,26 +861,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -536,11 +881,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -884,29 +1229,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2:Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -932,13 +1278,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>5</v>
@@ -947,78 +1293,85 @@
         <v>6</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="S1" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="Y1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>40526073209</v>
-      </c>
-      <c r="B2" s="1">
-        <v>4507923175</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>32</v>
+      <c r="A2" s="12">
+        <v>40556665829</v>
+      </c>
+      <c r="B2" s="12">
+        <v>4542691818</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="K2" s="13">
+        <v>0</v>
+      </c>
       <c r="L2">
         <v>1</v>
       </c>
@@ -1035,13 +1388,13 @@
         <v>6</v>
       </c>
       <c r="Q2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -1057,7 +1410,7 @@
       </c>
       <c r="Y2" s="1">
         <f t="shared" ref="Y2" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Z2" s="1">
         <f t="shared" ref="Z2" si="1">VLOOKUP(H2,T_TIPO_ENVIO,2,FALSE)</f>
@@ -1065,26 +1418,35 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>40525343765</v>
-      </c>
-      <c r="B3" s="1">
-        <v>4507112075</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>32</v>
+      <c r="A3" s="12">
+        <v>40556382310</v>
+      </c>
+      <c r="B3" s="12">
+        <v>4542372833</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
@@ -1102,18 +1464,17 @@
         <v>6</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
       </c>
-      <c r="U3" s="1"/>
       <c r="V3" s="1">
         <v>0</v>
       </c>
@@ -1125,7 +1486,7 @@
       </c>
       <c r="Y3" s="1">
         <f t="shared" ref="Y3:Y4" si="2">VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Z3" s="1">
         <f t="shared" ref="Z3:Z4" si="3">VLOOKUP(H3,T_TIPO_ENVIO,2,FALSE)</f>
@@ -1133,26 +1494,35 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>40525088347</v>
-      </c>
-      <c r="B4">
-        <v>4506811206</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
+      <c r="A4" s="12">
+        <v>40556363399</v>
+      </c>
+      <c r="B4" s="12">
+        <v>4542352793</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
@@ -1170,13 +1540,13 @@
         <v>6</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T4" s="1">
         <v>0</v>
@@ -1193,7 +1563,7 @@
       </c>
       <c r="Y4" s="1">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Z4" s="1">
         <f t="shared" si="3"/>
@@ -1201,26 +1571,35 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>40525040749</v>
-      </c>
-      <c r="B5">
-        <v>4506754594</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
+      <c r="A5" s="12">
+        <v>40556312249</v>
+      </c>
+      <c r="B5" s="12">
+        <v>4542295424</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>1</v>
@@ -1238,13 +1617,13 @@
         <v>6</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T5" s="1">
         <v>0</v>
@@ -1260,59 +1639,527 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <f t="shared" ref="Y5" si="4">VLOOKUP(E5,T_OPERADORES,2,FALSE)</f>
-        <v>7</v>
+        <f t="shared" ref="Y5:Y9" si="4">VLOOKUP(E5,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="Z5" s="1">
-        <f t="shared" ref="Z5" si="5">VLOOKUP(H5,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="Z5:Z9" si="5">VLOOKUP(H5,T_TIPO_ENVIO,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>40555549504</v>
+      </c>
+      <c r="B6" s="12">
+        <v>4541427252</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="K6" s="13">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>17</v>
+      </c>
+      <c r="O6" s="1">
+        <v>20</v>
+      </c>
+      <c r="P6" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1"/>
+      <c r="V6" s="10">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <v>3</v>
+      </c>
+      <c r="X6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="Z6" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>40555485116</v>
+      </c>
+      <c r="B7" s="12">
+        <v>4541351503</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" s="13">
+        <v>0</v>
+      </c>
+      <c r="L7" s="13">
+        <v>1</v>
+      </c>
+      <c r="M7" s="13">
+        <v>1</v>
+      </c>
+      <c r="N7" s="13">
+        <v>17</v>
+      </c>
+      <c r="O7" s="13">
+        <v>20</v>
+      </c>
+      <c r="P7" s="13">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="13">
+        <v>0</v>
+      </c>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13">
+        <v>0</v>
+      </c>
+      <c r="W7" s="13">
+        <v>3</v>
+      </c>
+      <c r="X7" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="Z7" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>40555468807</v>
+      </c>
+      <c r="B8" s="12">
+        <v>4541333239</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0</v>
+      </c>
+      <c r="L8" s="13">
+        <v>1</v>
+      </c>
+      <c r="M8" s="13">
+        <v>1</v>
+      </c>
+      <c r="N8" s="13">
+        <v>17</v>
+      </c>
+      <c r="O8" s="13">
+        <v>20</v>
+      </c>
+      <c r="P8" s="13">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="T8" s="13">
+        <v>0</v>
+      </c>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13">
+        <v>0</v>
+      </c>
+      <c r="W8" s="13">
+        <v>3</v>
+      </c>
+      <c r="X8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="Z8" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>40554940145</v>
+      </c>
+      <c r="B9" s="12">
+        <v>4540736244</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="12">
+        <v>1</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="13">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13">
+        <v>1</v>
+      </c>
+      <c r="M9" s="13">
+        <v>1</v>
+      </c>
+      <c r="N9" s="13">
+        <v>17</v>
+      </c>
+      <c r="O9" s="13">
+        <v>20</v>
+      </c>
+      <c r="P9" s="13">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="T9" s="13">
+        <v>0</v>
+      </c>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13">
+        <v>0</v>
+      </c>
+      <c r="W9" s="13">
+        <v>3</v>
+      </c>
+      <c r="X9" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="Z9" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>40554303905</v>
+      </c>
+      <c r="B10" s="12">
+        <v>4540017995</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="12">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="K10" s="13">
+        <v>0</v>
+      </c>
+      <c r="L10" s="13">
+        <v>1</v>
+      </c>
+      <c r="M10" s="13">
+        <v>1</v>
+      </c>
+      <c r="N10" s="13">
+        <v>17</v>
+      </c>
+      <c r="O10" s="13">
+        <v>20</v>
+      </c>
+      <c r="P10" s="13">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" s="13">
+        <v>0</v>
+      </c>
+      <c r="U10" s="13"/>
+      <c r="V10" s="10">
+        <v>0</v>
+      </c>
+      <c r="W10" s="10">
+        <v>3</v>
+      </c>
+      <c r="X10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="13">
+        <f t="shared" ref="Y10:Y11" si="6">VLOOKUP(E10,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="Z10" s="13">
+        <f t="shared" ref="Z10:Z11" si="7">VLOOKUP(H10,T_TIPO_ENVIO,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>4536771916</v>
+      </c>
+      <c r="B11" s="12">
+        <v>4536771916</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="12">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="K11" s="13">
+        <v>4536771916</v>
+      </c>
+      <c r="L11" s="13">
+        <v>1</v>
+      </c>
+      <c r="M11" s="13">
+        <v>1</v>
+      </c>
+      <c r="N11" s="13">
+        <v>17</v>
+      </c>
+      <c r="O11" s="13">
+        <v>20</v>
+      </c>
+      <c r="P11" s="13">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" s="13">
+        <v>0</v>
+      </c>
+      <c r="U11" s="13"/>
+      <c r="V11" s="10">
+        <v>0</v>
+      </c>
+      <c r="W11" s="13">
+        <v>3</v>
+      </c>
+      <c r="X11" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="13">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="Z11" s="13">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="duplicateValues" dxfId="16" priority="336"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="461"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="371"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="13" priority="555"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C1048576">
-    <cfRule type="duplicateValues" dxfId="12" priority="565"/>
+  <conditionalFormatting sqref="C4:C1048576">
+    <cfRule type="duplicateValues" dxfId="14" priority="456"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="11" priority="333"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="464"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="10" priority="334"/>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="12" priority="82"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="1053"/>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="11" priority="83"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="1056"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1 B4:B1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="1059"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="1062"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1 B4:B1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="1065"/>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="10" priority="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="4" priority="1068"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="64"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="8" priority="61"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="7" priority="62"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="6" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="3" priority="1069"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="65"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="2" priority="1070"/>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="4" priority="66"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="1" priority="1071"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="829"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="0" priority="1072"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="832"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1 A4:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="835"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1 A4:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="839"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1325,7 +2172,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,7 +2187,7 @@
       </c>
       <c r="B1" s="11"/>
       <c r="D1" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="11"/>
     </row>
@@ -1352,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1366,7 +2213,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -1379,10 +2226,16 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -1390,7 +2243,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -1398,7 +2251,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -1406,7 +2259,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1424,116 +2277,838 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A2:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K2" sqref="K2:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>40526228190</v>
+      </c>
+      <c r="B2">
+        <v>4508096248</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2">
+        <v>40526228190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>40526099231</v>
+      </c>
+      <c r="B3">
+        <v>4507948980</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3">
+        <v>40526099231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>40525111738</v>
+      </c>
+      <c r="B4">
+        <v>4506837014</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4">
+        <v>40525111738</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40525033754</v>
+      </c>
+      <c r="B5">
+        <v>4506748101</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5">
+        <v>40525033754</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>40524875384</v>
+      </c>
+      <c r="B7">
+        <v>4506562941</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M7">
+        <v>40524875384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>40524530482</v>
+      </c>
+      <c r="B8">
+        <v>4506172345</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8">
+        <v>40524530482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>40524236350</v>
+      </c>
+      <c r="B9">
+        <v>4505834791</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9">
+        <v>40524236350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>40524094587</v>
+      </c>
+      <c r="B10">
+        <v>4505666961</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10">
+        <v>40524094587</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>40524032095</v>
+      </c>
+      <c r="B13">
+        <v>4505604636</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13">
+        <v>40524032095</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>40523993572</v>
+      </c>
+      <c r="B14">
+        <v>4505562076</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14">
+        <v>40523993572</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>40523886241</v>
+      </c>
+      <c r="B15">
+        <v>4505439684</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="7">
+        <v>44305</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" t="s">
+        <v>73</v>
+      </c>
+      <c r="M15">
+        <v>40523886241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>40523340733</v>
+      </c>
+      <c r="B16">
+        <v>4504809746</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K16" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16">
+        <v>40523340733</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>40523241897</v>
+      </c>
+      <c r="B17">
+        <v>4504703265</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K17" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" t="s">
+        <v>78</v>
+      </c>
+      <c r="M17">
+        <v>40523241897</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>40522955816</v>
+      </c>
+      <c r="B18">
+        <v>4504374865</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K18" t="s">
+        <v>79</v>
+      </c>
+      <c r="L18" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18">
+        <v>40522955816</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>40522913732</v>
+      </c>
+      <c r="B19">
+        <v>4504331038</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="7">
+        <v>44305</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="K19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L19" t="s">
+        <v>83</v>
+      </c>
+      <c r="M19">
+        <v>40522913732</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>40522510981</v>
+      </c>
+      <c r="B20">
+        <v>4503863956</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K20" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M20">
+        <v>40522510981</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>40522422562</v>
+      </c>
+      <c r="B21">
+        <v>4503771756</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K21" t="s">
+        <v>88</v>
+      </c>
+      <c r="L21" t="s">
+        <v>89</v>
+      </c>
+      <c r="M21">
+        <v>40522422562</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>40522024735</v>
+      </c>
+      <c r="B22">
+        <v>4503316316</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K22" t="s">
+        <v>91</v>
+      </c>
+      <c r="L22" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22">
+        <v>40522024735</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>40522022735</v>
+      </c>
+      <c r="B23">
+        <v>4503313791</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K23" t="s">
+        <v>93</v>
+      </c>
+      <c r="L23" t="s">
+        <v>94</v>
+      </c>
+      <c r="M23">
+        <v>40522022735</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>40521479578</v>
+      </c>
+      <c r="B24">
+        <v>4502696901</v>
+      </c>
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K24" t="s">
+        <v>96</v>
+      </c>
+      <c r="L24" t="s">
+        <v>97</v>
+      </c>
+      <c r="M24">
+        <v>40521479578</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>40521433878</v>
+      </c>
+      <c r="B25">
+        <v>4502640970</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K25" t="s">
+        <v>98</v>
+      </c>
+      <c r="L25" t="s">
+        <v>99</v>
+      </c>
+      <c r="M25">
+        <v>40521433878</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>40521373894</v>
+      </c>
+      <c r="B26">
+        <v>4502581372</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K26" t="s">
+        <v>101</v>
+      </c>
+      <c r="L26" t="s">
+        <v>102</v>
+      </c>
+      <c r="M26">
+        <v>40521373894</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2120</v>
+      </c>
+      <c r="C27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K27" t="s">
+        <v>104</v>
+      </c>
+      <c r="L27" t="s">
+        <v>105</v>
+      </c>
+      <c r="M27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="7">
+        <v>44305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>2113</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K29" t="s">
+        <v>109</v>
+      </c>
+      <c r="L29" t="s">
+        <v>110</v>
+      </c>
+      <c r="M29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>40526518865</v>
+      </c>
+      <c r="B30">
+        <v>4508423565</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K30" t="s">
+        <v>112</v>
+      </c>
+      <c r="L30" t="s">
+        <v>113</v>
+      </c>
+      <c r="M30">
+        <v>40526518865</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>40516953732</v>
+      </c>
+      <c r="B31">
+        <v>4497572116</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="7">
+        <v>44305</v>
+      </c>
+      <c r="K31" t="s">
+        <v>114</v>
+      </c>
+      <c r="L31" t="s">
+        <v>115</v>
+      </c>
+      <c r="M31">
+        <v>40516953732</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
@@ -1541,24 +3116,6 @@
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>